<commit_message>
Update seed with more user data
</commit_message>
<xml_diff>
--- a/src/data/seed.xlsx
+++ b/src/data/seed.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="18110"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8020" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Account" sheetId="1" r:id="rId1"/>
@@ -26,6 +26,9 @@
     <sheet name="ContainsPart" sheetId="12" r:id="rId12"/>
     <sheet name="RatesVendor" sheetId="13" r:id="rId13"/>
   </sheets>
+  <definedNames>
+    <definedName name="MOCK_DATA__2" localSheetId="0">Account!$A$2:$L$21</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -35,8 +38,31 @@
 </workbook>
 </file>
 
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="MOCK_DATA (2)" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="850" sourceFile="C:\Users\Scott\Downloads\Browser\MOCK_DATA (2).csv" comma="1">
+      <textFields count="12">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+</connections>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="201">
   <si>
     <t>customerId</t>
   </si>
@@ -188,49 +214,467 @@
     <t>admin</t>
   </si>
   <si>
-    <t>joe@test.com</t>
-  </si>
-  <si>
-    <t>pswd</t>
-  </si>
-  <si>
-    <t>joe</t>
-  </si>
-  <si>
-    <t>shmoe</t>
-  </si>
-  <si>
-    <t>1234 Fake St</t>
-  </si>
-  <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>Province</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>A1A1A1</t>
+    <t>vendor</t>
+  </si>
+  <si>
+    <t>customer</t>
+  </si>
+  <si>
+    <t>dcoleman0@gravatar.com</t>
+  </si>
+  <si>
+    <t>nec</t>
+  </si>
+  <si>
+    <t>Doris</t>
+  </si>
+  <si>
+    <t>Coleman</t>
+  </si>
+  <si>
+    <t>1-(202)876-8809</t>
+  </si>
+  <si>
+    <t>0475 Cambridge Parkway</t>
+  </si>
+  <si>
+    <t>Washington</t>
+  </si>
+  <si>
+    <t>District of Columbia</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>ghawkins1@yelp.com</t>
+  </si>
+  <si>
+    <t>vivamus</t>
+  </si>
+  <si>
+    <t>Gary</t>
+  </si>
+  <si>
+    <t>Hawkins</t>
+  </si>
+  <si>
+    <t>1-(518)163-8665</t>
+  </si>
+  <si>
+    <t>22868 Forest Place</t>
+  </si>
+  <si>
+    <t>Albany</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>emiller2@chicagotribune.com</t>
+  </si>
+  <si>
+    <t>ligula</t>
+  </si>
+  <si>
+    <t>Eugene</t>
+  </si>
+  <si>
+    <t>Miller</t>
+  </si>
+  <si>
+    <t>1-(518)661-6997</t>
+  </si>
+  <si>
+    <t>5 Lerdahl Road</t>
+  </si>
+  <si>
+    <t>mhawkins3@shinystat.com</t>
+  </si>
+  <si>
+    <t>porttitor</t>
+  </si>
+  <si>
+    <t>Marilyn</t>
+  </si>
+  <si>
+    <t>1-(305)863-3025</t>
+  </si>
+  <si>
+    <t>8125 Oriole Parkway</t>
+  </si>
+  <si>
+    <t>Miami</t>
+  </si>
+  <si>
+    <t>Florida</t>
+  </si>
+  <si>
+    <t>mprice4@mediafire.com</t>
+  </si>
+  <si>
+    <t>faucibus</t>
+  </si>
+  <si>
+    <t>Maria</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>1-(202)146-8119</t>
+  </si>
+  <si>
+    <t>48 Heath Plaza</t>
+  </si>
+  <si>
+    <t>mcrawford5@tripod.com</t>
+  </si>
+  <si>
+    <t>pellentesque</t>
+  </si>
+  <si>
+    <t>Mary</t>
+  </si>
+  <si>
+    <t>Crawford</t>
+  </si>
+  <si>
+    <t>1-(561)147-4896</t>
+  </si>
+  <si>
+    <t>0 Spenser Park</t>
+  </si>
+  <si>
+    <t>Lake Worth</t>
+  </si>
+  <si>
+    <t>ecooper6@mlb.com</t>
+  </si>
+  <si>
+    <t>cubilia</t>
+  </si>
+  <si>
+    <t>Ernest</t>
+  </si>
+  <si>
+    <t>Cooper</t>
+  </si>
+  <si>
+    <t>1-(214)687-7486</t>
+  </si>
+  <si>
+    <t>56 Sachs Terrace</t>
+  </si>
+  <si>
+    <t>Garland</t>
+  </si>
+  <si>
+    <t>Texas</t>
+  </si>
+  <si>
+    <t>cmarshall7@topsy.com</t>
+  </si>
+  <si>
+    <t>semper</t>
+  </si>
+  <si>
+    <t>Carol</t>
+  </si>
+  <si>
+    <t>Marshall</t>
+  </si>
+  <si>
+    <t>1-(251)323-3089</t>
+  </si>
+  <si>
+    <t>03694 Starling Trail</t>
+  </si>
+  <si>
+    <t>Mobile</t>
+  </si>
+  <si>
+    <t>Alabama</t>
+  </si>
+  <si>
+    <t>jmartin8@java.com</t>
+  </si>
+  <si>
+    <t>gravida</t>
+  </si>
+  <si>
+    <t>Jacqueline</t>
+  </si>
+  <si>
+    <t>Martin</t>
+  </si>
+  <si>
+    <t>1-(701)240-4735</t>
+  </si>
+  <si>
+    <t>28227 Badeau Parkway</t>
+  </si>
+  <si>
+    <t>Fargo</t>
+  </si>
+  <si>
+    <t>North Dakota</t>
+  </si>
+  <si>
+    <t>rflores9@economist.com</t>
+  </si>
+  <si>
+    <t>diam</t>
+  </si>
+  <si>
+    <t>Robin</t>
+  </si>
+  <si>
+    <t>Flores</t>
+  </si>
+  <si>
+    <t>1-(608)357-6583</t>
+  </si>
+  <si>
+    <t>77700 Forest Place</t>
+  </si>
+  <si>
+    <t>Madison</t>
+  </si>
+  <si>
+    <t>Wisconsin</t>
+  </si>
+  <si>
+    <t>rshawa@tamu.edu</t>
+  </si>
+  <si>
+    <t>mus</t>
+  </si>
+  <si>
+    <t>Rebecca</t>
+  </si>
+  <si>
+    <t>Shaw</t>
+  </si>
+  <si>
+    <t>1-(520)347-5517</t>
+  </si>
+  <si>
+    <t>8190 Center Place</t>
+  </si>
+  <si>
+    <t>Tucson</t>
+  </si>
+  <si>
+    <t>Arizona</t>
+  </si>
+  <si>
+    <t>jdanielsb@imgur.com</t>
+  </si>
+  <si>
+    <t>augue</t>
+  </si>
+  <si>
+    <t>Johnny</t>
+  </si>
+  <si>
+    <t>Daniels</t>
+  </si>
+  <si>
+    <t>1-(731)828-9905</t>
+  </si>
+  <si>
+    <t>5550 Sachs Drive</t>
+  </si>
+  <si>
+    <t>Jackson</t>
+  </si>
+  <si>
+    <t>Tennessee</t>
+  </si>
+  <si>
+    <t>redwardsc@jiathis.com</t>
+  </si>
+  <si>
+    <t>Ruby</t>
+  </si>
+  <si>
+    <t>Edwards</t>
+  </si>
+  <si>
+    <t>1-(513)194-4635</t>
+  </si>
+  <si>
+    <t>38 Petterle Street</t>
+  </si>
+  <si>
+    <t>Cincinnati</t>
+  </si>
+  <si>
+    <t>Ohio</t>
+  </si>
+  <si>
+    <t>cmyersd@nifty.com</t>
+  </si>
+  <si>
+    <t>curabitur</t>
+  </si>
+  <si>
+    <t>Carl</t>
+  </si>
+  <si>
+    <t>Myers</t>
+  </si>
+  <si>
+    <t>1-(608)855-1945</t>
+  </si>
+  <si>
+    <t>666 Burrows Junction</t>
+  </si>
+  <si>
+    <t>pcolee@sourceforge.net</t>
+  </si>
+  <si>
+    <t>sapien</t>
+  </si>
+  <si>
+    <t>Patricia</t>
+  </si>
+  <si>
+    <t>Cole</t>
+  </si>
+  <si>
+    <t>1-(717)176-0760</t>
+  </si>
+  <si>
+    <t>2690 Sundown Terrace</t>
+  </si>
+  <si>
+    <t>Lancaster</t>
+  </si>
+  <si>
+    <t>Pennsylvania</t>
+  </si>
+  <si>
+    <t>jwarrenf@theglobeandmail.com</t>
+  </si>
+  <si>
+    <t>primis</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Warren</t>
+  </si>
+  <si>
+    <t>1-(304)702-9618</t>
+  </si>
+  <si>
+    <t>366 School Terrace</t>
+  </si>
+  <si>
+    <t>Huntington</t>
+  </si>
+  <si>
+    <t>West Virginia</t>
+  </si>
+  <si>
+    <t>ffoxg@economist.com</t>
+  </si>
+  <si>
+    <t>Fred</t>
+  </si>
+  <si>
+    <t>Fox</t>
+  </si>
+  <si>
+    <t>1-(757)220-7707</t>
+  </si>
+  <si>
+    <t>4 Porter Trail</t>
+  </si>
+  <si>
+    <t>Norfolk</t>
+  </si>
+  <si>
+    <t>Virginia</t>
+  </si>
+  <si>
+    <t>pharrish@comsenz.com</t>
+  </si>
+  <si>
+    <t>pharetra</t>
+  </si>
+  <si>
+    <t>Phillip</t>
+  </si>
+  <si>
+    <t>Harris</t>
+  </si>
+  <si>
+    <t>1-(650)359-8512</t>
+  </si>
+  <si>
+    <t>0 Thierer Place</t>
+  </si>
+  <si>
+    <t>Redwood City</t>
+  </si>
+  <si>
+    <t>California</t>
+  </si>
+  <si>
+    <t>scolei@theguardian.com</t>
+  </si>
+  <si>
+    <t>morbi</t>
+  </si>
+  <si>
+    <t>Scott</t>
+  </si>
+  <si>
+    <t>1-(951)303-0657</t>
+  </si>
+  <si>
+    <t>78 Jay Terrace</t>
+  </si>
+  <si>
+    <t>Corona</t>
+  </si>
+  <si>
+    <t>gfowlerj@slashdot.org</t>
+  </si>
+  <si>
+    <t>proin</t>
+  </si>
+  <si>
+    <t>Gerald</t>
+  </si>
+  <si>
+    <t>Fowler</t>
+  </si>
+  <si>
+    <t>1-(515)167-4752</t>
+  </si>
+  <si>
+    <t>396 Maple Wood Place</t>
+  </si>
+  <si>
+    <t>Des Moines</t>
+  </si>
+  <si>
+    <t>Iowa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -253,16 +697,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -276,6 +717,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MOCK_DATA (2)" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -541,26 +986,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.08984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="3.6328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.6328125" customWidth="1"/>
+    <col min="7" max="7" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.81640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.7265625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="3.6328125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
@@ -608,41 +1065,760 @@
       <c r="B2" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I2" t="s">
+        <v>58</v>
+      </c>
+      <c r="J2" t="s">
+        <v>59</v>
+      </c>
+      <c r="K2" t="s">
+        <v>60</v>
+      </c>
+      <c r="L2">
+        <v>20057</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G3" t="s">
+        <v>65</v>
+      </c>
+      <c r="H3" t="s">
+        <v>66</v>
+      </c>
+      <c r="I3" t="s">
+        <v>67</v>
+      </c>
+      <c r="J3" t="s">
+        <v>68</v>
+      </c>
+      <c r="K3" t="s">
+        <v>60</v>
+      </c>
+      <c r="L3">
+        <v>12255</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>50</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H4" t="s">
+        <v>74</v>
+      </c>
+      <c r="I4" t="s">
+        <v>67</v>
+      </c>
+      <c r="J4" t="s">
+        <v>68</v>
+      </c>
+      <c r="K4" t="s">
+        <v>60</v>
+      </c>
+      <c r="L4">
+        <v>12237</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>51</v>
       </c>
-      <c r="E2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F2" t="s">
-        <v>53</v>
-      </c>
-      <c r="G2">
-        <v>1234567890</v>
-      </c>
-      <c r="H2" t="s">
-        <v>54</v>
-      </c>
-      <c r="I2" t="s">
-        <v>55</v>
-      </c>
-      <c r="J2" t="s">
-        <v>56</v>
-      </c>
-      <c r="K2" t="s">
-        <v>57</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="C5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E5" t="s">
+        <v>77</v>
+      </c>
+      <c r="F5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G5" t="s">
+        <v>78</v>
+      </c>
+      <c r="H5" t="s">
+        <v>79</v>
+      </c>
+      <c r="I5" t="s">
+        <v>80</v>
+      </c>
+      <c r="J5" t="s">
+        <v>81</v>
+      </c>
+      <c r="K5" t="s">
+        <v>60</v>
+      </c>
+      <c r="L5">
+        <v>33185</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E6" t="s">
+        <v>84</v>
+      </c>
+      <c r="F6" t="s">
+        <v>85</v>
+      </c>
+      <c r="G6" t="s">
+        <v>86</v>
+      </c>
+      <c r="H6" t="s">
+        <v>87</v>
+      </c>
+      <c r="I6" t="s">
         <v>58</v>
       </c>
+      <c r="J6" t="s">
+        <v>59</v>
+      </c>
+      <c r="K6" t="s">
+        <v>60</v>
+      </c>
+      <c r="L6">
+        <v>20022</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7" t="s">
+        <v>89</v>
+      </c>
+      <c r="E7" t="s">
+        <v>90</v>
+      </c>
+      <c r="F7" t="s">
+        <v>91</v>
+      </c>
+      <c r="G7" t="s">
+        <v>92</v>
+      </c>
+      <c r="H7" t="s">
+        <v>93</v>
+      </c>
+      <c r="I7" t="s">
+        <v>94</v>
+      </c>
+      <c r="J7" t="s">
+        <v>81</v>
+      </c>
+      <c r="K7" t="s">
+        <v>60</v>
+      </c>
+      <c r="L7">
+        <v>33467</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" t="s">
+        <v>95</v>
+      </c>
+      <c r="D8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E8" t="s">
+        <v>97</v>
+      </c>
+      <c r="F8" t="s">
+        <v>98</v>
+      </c>
+      <c r="G8" t="s">
+        <v>99</v>
+      </c>
+      <c r="H8" t="s">
+        <v>100</v>
+      </c>
+      <c r="I8" t="s">
+        <v>101</v>
+      </c>
+      <c r="J8" t="s">
+        <v>102</v>
+      </c>
+      <c r="K8" t="s">
+        <v>60</v>
+      </c>
+      <c r="L8">
+        <v>75049</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" t="s">
+        <v>103</v>
+      </c>
+      <c r="D9" t="s">
+        <v>104</v>
+      </c>
+      <c r="E9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F9" t="s">
+        <v>106</v>
+      </c>
+      <c r="G9" t="s">
+        <v>107</v>
+      </c>
+      <c r="H9" t="s">
+        <v>108</v>
+      </c>
+      <c r="I9" t="s">
+        <v>109</v>
+      </c>
+      <c r="J9" t="s">
+        <v>110</v>
+      </c>
+      <c r="K9" t="s">
+        <v>60</v>
+      </c>
+      <c r="L9">
+        <v>36622</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" t="s">
+        <v>111</v>
+      </c>
+      <c r="D10" t="s">
+        <v>112</v>
+      </c>
+      <c r="E10" t="s">
+        <v>113</v>
+      </c>
+      <c r="F10" t="s">
+        <v>114</v>
+      </c>
+      <c r="G10" t="s">
+        <v>115</v>
+      </c>
+      <c r="H10" t="s">
+        <v>116</v>
+      </c>
+      <c r="I10" t="s">
+        <v>117</v>
+      </c>
+      <c r="J10" t="s">
+        <v>118</v>
+      </c>
+      <c r="K10" t="s">
+        <v>60</v>
+      </c>
+      <c r="L10">
+        <v>58122</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" t="s">
+        <v>119</v>
+      </c>
+      <c r="D11" t="s">
+        <v>120</v>
+      </c>
+      <c r="E11" t="s">
+        <v>121</v>
+      </c>
+      <c r="F11" t="s">
+        <v>122</v>
+      </c>
+      <c r="G11" t="s">
+        <v>123</v>
+      </c>
+      <c r="H11" t="s">
+        <v>124</v>
+      </c>
+      <c r="I11" t="s">
+        <v>125</v>
+      </c>
+      <c r="J11" t="s">
+        <v>126</v>
+      </c>
+      <c r="K11" t="s">
+        <v>60</v>
+      </c>
+      <c r="L11">
+        <v>53779</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" t="s">
+        <v>127</v>
+      </c>
+      <c r="D12" t="s">
+        <v>128</v>
+      </c>
+      <c r="E12" t="s">
+        <v>129</v>
+      </c>
+      <c r="F12" t="s">
+        <v>130</v>
+      </c>
+      <c r="G12" t="s">
+        <v>131</v>
+      </c>
+      <c r="H12" t="s">
+        <v>132</v>
+      </c>
+      <c r="I12" t="s">
+        <v>133</v>
+      </c>
+      <c r="J12" t="s">
+        <v>134</v>
+      </c>
+      <c r="K12" t="s">
+        <v>60</v>
+      </c>
+      <c r="L12">
+        <v>85715</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" t="s">
+        <v>135</v>
+      </c>
+      <c r="D13" t="s">
+        <v>136</v>
+      </c>
+      <c r="E13" t="s">
+        <v>137</v>
+      </c>
+      <c r="F13" t="s">
+        <v>138</v>
+      </c>
+      <c r="G13" t="s">
+        <v>139</v>
+      </c>
+      <c r="H13" t="s">
+        <v>140</v>
+      </c>
+      <c r="I13" t="s">
+        <v>141</v>
+      </c>
+      <c r="J13" t="s">
+        <v>142</v>
+      </c>
+      <c r="K13" t="s">
+        <v>60</v>
+      </c>
+      <c r="L13">
+        <v>38308</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" t="s">
+        <v>143</v>
+      </c>
+      <c r="D14" t="s">
+        <v>89</v>
+      </c>
+      <c r="E14" t="s">
+        <v>144</v>
+      </c>
+      <c r="F14" t="s">
+        <v>145</v>
+      </c>
+      <c r="G14" t="s">
+        <v>146</v>
+      </c>
+      <c r="H14" t="s">
+        <v>147</v>
+      </c>
+      <c r="I14" t="s">
+        <v>148</v>
+      </c>
+      <c r="J14" t="s">
+        <v>149</v>
+      </c>
+      <c r="K14" t="s">
+        <v>60</v>
+      </c>
+      <c r="L14">
+        <v>45271</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" t="s">
+        <v>150</v>
+      </c>
+      <c r="D15" t="s">
+        <v>151</v>
+      </c>
+      <c r="E15" t="s">
+        <v>152</v>
+      </c>
+      <c r="F15" t="s">
+        <v>153</v>
+      </c>
+      <c r="G15" t="s">
+        <v>154</v>
+      </c>
+      <c r="H15" t="s">
+        <v>155</v>
+      </c>
+      <c r="I15" t="s">
+        <v>125</v>
+      </c>
+      <c r="J15" t="s">
+        <v>126</v>
+      </c>
+      <c r="K15" t="s">
+        <v>60</v>
+      </c>
+      <c r="L15">
+        <v>53710</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" t="s">
+        <v>156</v>
+      </c>
+      <c r="D16" t="s">
+        <v>157</v>
+      </c>
+      <c r="E16" t="s">
+        <v>158</v>
+      </c>
+      <c r="F16" t="s">
+        <v>159</v>
+      </c>
+      <c r="G16" t="s">
+        <v>160</v>
+      </c>
+      <c r="H16" t="s">
+        <v>161</v>
+      </c>
+      <c r="I16" t="s">
+        <v>162</v>
+      </c>
+      <c r="J16" t="s">
+        <v>163</v>
+      </c>
+      <c r="K16" t="s">
+        <v>60</v>
+      </c>
+      <c r="L16">
+        <v>17622</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" t="s">
+        <v>164</v>
+      </c>
+      <c r="D17" t="s">
+        <v>165</v>
+      </c>
+      <c r="E17" t="s">
+        <v>166</v>
+      </c>
+      <c r="F17" t="s">
+        <v>167</v>
+      </c>
+      <c r="G17" t="s">
+        <v>168</v>
+      </c>
+      <c r="H17" t="s">
+        <v>169</v>
+      </c>
+      <c r="I17" t="s">
+        <v>170</v>
+      </c>
+      <c r="J17" t="s">
+        <v>171</v>
+      </c>
+      <c r="K17" t="s">
+        <v>60</v>
+      </c>
+      <c r="L17">
+        <v>25775</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" t="s">
+        <v>172</v>
+      </c>
+      <c r="D18" t="s">
+        <v>83</v>
+      </c>
+      <c r="E18" t="s">
+        <v>173</v>
+      </c>
+      <c r="F18" t="s">
+        <v>174</v>
+      </c>
+      <c r="G18" t="s">
+        <v>175</v>
+      </c>
+      <c r="H18" t="s">
+        <v>176</v>
+      </c>
+      <c r="I18" t="s">
+        <v>177</v>
+      </c>
+      <c r="J18" t="s">
+        <v>178</v>
+      </c>
+      <c r="K18" t="s">
+        <v>60</v>
+      </c>
+      <c r="L18">
+        <v>23514</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" t="s">
+        <v>179</v>
+      </c>
+      <c r="D19" t="s">
+        <v>180</v>
+      </c>
+      <c r="E19" t="s">
+        <v>181</v>
+      </c>
+      <c r="F19" t="s">
+        <v>182</v>
+      </c>
+      <c r="G19" t="s">
+        <v>183</v>
+      </c>
+      <c r="H19" t="s">
+        <v>184</v>
+      </c>
+      <c r="I19" t="s">
+        <v>185</v>
+      </c>
+      <c r="J19" t="s">
+        <v>186</v>
+      </c>
+      <c r="K19" t="s">
+        <v>60</v>
+      </c>
+      <c r="L19">
+        <v>94064</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" t="s">
+        <v>187</v>
+      </c>
+      <c r="D20" t="s">
+        <v>188</v>
+      </c>
+      <c r="E20" t="s">
+        <v>189</v>
+      </c>
+      <c r="F20" t="s">
+        <v>159</v>
+      </c>
+      <c r="G20" t="s">
+        <v>190</v>
+      </c>
+      <c r="H20" t="s">
+        <v>191</v>
+      </c>
+      <c r="I20" t="s">
+        <v>192</v>
+      </c>
+      <c r="J20" t="s">
+        <v>186</v>
+      </c>
+      <c r="K20" t="s">
+        <v>60</v>
+      </c>
+      <c r="L20">
+        <v>92878</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" t="s">
+        <v>193</v>
+      </c>
+      <c r="D21" t="s">
+        <v>194</v>
+      </c>
+      <c r="E21" t="s">
+        <v>195</v>
+      </c>
+      <c r="F21" t="s">
+        <v>196</v>
+      </c>
+      <c r="G21" t="s">
+        <v>197</v>
+      </c>
+      <c r="H21" t="s">
+        <v>198</v>
+      </c>
+      <c r="I21" t="s">
+        <v>199</v>
+      </c>
+      <c r="J21" t="s">
+        <v>200</v>
+      </c>
+      <c r="K21" t="s">
+        <v>60</v>
+      </c>
+      <c r="L21">
+        <v>50936</v>
+      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -845,16 +2021,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Update seed with small amount of part and category data
</commit_message>
<xml_diff>
--- a/src/data/seed.xlsx
+++ b/src/data/seed.xlsx
@@ -9,22 +9,22 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8020" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11140" windowHeight="2360" tabRatio="833" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Account" sheetId="1" r:id="rId1"/>
-    <sheet name="Part" sheetId="2" r:id="rId2"/>
-    <sheet name="PartCategory" sheetId="3" r:id="rId3"/>
-    <sheet name="Vehicle" sheetId="4" r:id="rId4"/>
-    <sheet name="Make" sheetId="5" r:id="rId5"/>
-    <sheet name="Model" sheetId="6" r:id="rId6"/>
-    <sheet name="Order" sheetId="7" r:id="rId7"/>
-    <sheet name="Shipment" sheetId="8" r:id="rId8"/>
-    <sheet name="Payment" sheetId="9" r:id="rId9"/>
-    <sheet name="ListedPart" sheetId="10" r:id="rId10"/>
-    <sheet name="FitsIn" sheetId="11" r:id="rId11"/>
-    <sheet name="ContainsPart" sheetId="12" r:id="rId12"/>
-    <sheet name="RatesVendor" sheetId="13" r:id="rId13"/>
+    <sheet name="RatesVendor" sheetId="13" r:id="rId2"/>
+    <sheet name="PartOrder" sheetId="7" r:id="rId3"/>
+    <sheet name="Payment" sheetId="9" r:id="rId4"/>
+    <sheet name="Shipment" sheetId="8" r:id="rId5"/>
+    <sheet name="PartCategory" sheetId="3" r:id="rId6"/>
+    <sheet name="Part" sheetId="2" r:id="rId7"/>
+    <sheet name="ListedPart" sheetId="10" r:id="rId8"/>
+    <sheet name="ContainsPart" sheetId="12" r:id="rId9"/>
+    <sheet name="Make" sheetId="5" r:id="rId10"/>
+    <sheet name="Model" sheetId="6" r:id="rId11"/>
+    <sheet name="Vehicle" sheetId="4" r:id="rId12"/>
+    <sheet name="FitsIn" sheetId="11" r:id="rId13"/>
   </sheets>
   <definedNames>
     <definedName name="MOCK_DATA__2" localSheetId="0">Account!$A$2:$L$21</definedName>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="207">
   <si>
     <t>customerId</t>
   </si>
@@ -172,9 +172,6 @@
     <t>partName</t>
   </si>
   <si>
-    <t>image</t>
-  </si>
-  <si>
     <t>accountId</t>
   </si>
   <si>
@@ -665,6 +662,27 @@
   </si>
   <si>
     <t>Iowa</t>
+  </si>
+  <si>
+    <t>dateListed</t>
+  </si>
+  <si>
+    <t>imagePath</t>
+  </si>
+  <si>
+    <t>Seat</t>
+  </si>
+  <si>
+    <t>Red/Black Seat</t>
+  </si>
+  <si>
+    <t>Red and black seat</t>
+  </si>
+  <si>
+    <t>Place to sit</t>
+  </si>
+  <si>
+    <t>public/images/parts/part1.jpg</t>
   </si>
 </sst>
 </file>
@@ -700,8 +718,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -989,7 +1008,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1022,40 +1041,40 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
         <v>37</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>38</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>39</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>40</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>41</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>42</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>43</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>44</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>45</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>46</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>47</v>
-      </c>
-      <c r="L1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
@@ -1063,34 +1082,34 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" t="s">
         <v>52</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>53</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>54</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>55</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>56</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>57</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>58</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>59</v>
-      </c>
-      <c r="K2" t="s">
-        <v>60</v>
       </c>
       <c r="L2">
         <v>20057</v>
@@ -1101,34 +1120,34 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" t="s">
         <v>61</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>62</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>63</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>64</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>65</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>66</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>67</v>
       </c>
-      <c r="J3" t="s">
-        <v>68</v>
-      </c>
       <c r="K3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L3">
         <v>12255</v>
@@ -1139,34 +1158,34 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" t="s">
         <v>69</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>70</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>71</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>72</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>73</v>
       </c>
-      <c r="H4" t="s">
-        <v>74</v>
-      </c>
       <c r="I4" t="s">
+        <v>66</v>
+      </c>
+      <c r="J4" t="s">
         <v>67</v>
       </c>
-      <c r="J4" t="s">
-        <v>68</v>
-      </c>
       <c r="K4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L4">
         <v>12237</v>
@@ -1177,34 +1196,34 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" t="s">
         <v>75</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>76</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" t="s">
         <v>77</v>
       </c>
-      <c r="F5" t="s">
-        <v>64</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>78</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>79</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>80</v>
       </c>
-      <c r="J5" t="s">
-        <v>81</v>
-      </c>
       <c r="K5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L5">
         <v>33185</v>
@@ -1215,34 +1234,34 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D6" t="s">
         <v>82</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>83</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>84</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>85</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>86</v>
       </c>
-      <c r="H6" t="s">
-        <v>87</v>
-      </c>
       <c r="I6" t="s">
+        <v>57</v>
+      </c>
+      <c r="J6" t="s">
         <v>58</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>59</v>
-      </c>
-      <c r="K6" t="s">
-        <v>60</v>
       </c>
       <c r="L6">
         <v>20022</v>
@@ -1253,34 +1272,34 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D7" t="s">
         <v>88</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>89</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>90</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>91</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>92</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>93</v>
       </c>
-      <c r="I7" t="s">
-        <v>94</v>
-      </c>
       <c r="J7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L7">
         <v>33467</v>
@@ -1291,34 +1310,34 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C8" t="s">
+        <v>94</v>
+      </c>
+      <c r="D8" t="s">
         <v>95</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>96</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>97</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>98</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>99</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>100</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>101</v>
       </c>
-      <c r="J8" t="s">
-        <v>102</v>
-      </c>
       <c r="K8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L8">
         <v>75049</v>
@@ -1329,34 +1348,34 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D9" t="s">
         <v>103</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>104</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>105</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>106</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>107</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>108</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>109</v>
       </c>
-      <c r="J9" t="s">
-        <v>110</v>
-      </c>
       <c r="K9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L9">
         <v>36622</v>
@@ -1367,34 +1386,34 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C10" t="s">
+        <v>110</v>
+      </c>
+      <c r="D10" t="s">
         <v>111</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>112</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>113</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>114</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>115</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>116</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>117</v>
       </c>
-      <c r="J10" t="s">
-        <v>118</v>
-      </c>
       <c r="K10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L10">
         <v>58122</v>
@@ -1405,34 +1424,34 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C11" t="s">
+        <v>118</v>
+      </c>
+      <c r="D11" t="s">
         <v>119</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>120</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>121</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>122</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>123</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>124</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>125</v>
       </c>
-      <c r="J11" t="s">
-        <v>126</v>
-      </c>
       <c r="K11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L11">
         <v>53779</v>
@@ -1443,34 +1462,34 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C12" t="s">
+        <v>126</v>
+      </c>
+      <c r="D12" t="s">
         <v>127</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>128</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>129</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>130</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>131</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>132</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>133</v>
       </c>
-      <c r="J12" t="s">
-        <v>134</v>
-      </c>
       <c r="K12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L12">
         <v>85715</v>
@@ -1481,34 +1500,34 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C13" t="s">
+        <v>134</v>
+      </c>
+      <c r="D13" t="s">
         <v>135</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>136</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>137</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>138</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>139</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>140</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>141</v>
       </c>
-      <c r="J13" t="s">
-        <v>142</v>
-      </c>
       <c r="K13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L13">
         <v>38308</v>
@@ -1519,34 +1538,34 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C14" t="s">
+        <v>142</v>
+      </c>
+      <c r="D14" t="s">
+        <v>88</v>
+      </c>
+      <c r="E14" t="s">
         <v>143</v>
       </c>
-      <c r="D14" t="s">
-        <v>89</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>144</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>145</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>146</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>147</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
         <v>148</v>
       </c>
-      <c r="J14" t="s">
-        <v>149</v>
-      </c>
       <c r="K14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L14">
         <v>45271</v>
@@ -1557,34 +1576,34 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C15" t="s">
+        <v>149</v>
+      </c>
+      <c r="D15" t="s">
         <v>150</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>151</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>152</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>153</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>154</v>
       </c>
-      <c r="H15" t="s">
-        <v>155</v>
-      </c>
       <c r="I15" t="s">
+        <v>124</v>
+      </c>
+      <c r="J15" t="s">
         <v>125</v>
       </c>
-      <c r="J15" t="s">
-        <v>126</v>
-      </c>
       <c r="K15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L15">
         <v>53710</v>
@@ -1595,34 +1614,34 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C16" t="s">
+        <v>155</v>
+      </c>
+      <c r="D16" t="s">
         <v>156</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>157</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>158</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>159</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>160</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
         <v>161</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" t="s">
         <v>162</v>
       </c>
-      <c r="J16" t="s">
-        <v>163</v>
-      </c>
       <c r="K16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L16">
         <v>17622</v>
@@ -1633,34 +1652,34 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C17" t="s">
+        <v>163</v>
+      </c>
+      <c r="D17" t="s">
         <v>164</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>165</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>166</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>167</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>168</v>
       </c>
-      <c r="H17" t="s">
+      <c r="I17" t="s">
         <v>169</v>
       </c>
-      <c r="I17" t="s">
+      <c r="J17" t="s">
         <v>170</v>
       </c>
-      <c r="J17" t="s">
-        <v>171</v>
-      </c>
       <c r="K17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L17">
         <v>25775</v>
@@ -1671,34 +1690,34 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C18" t="s">
+        <v>171</v>
+      </c>
+      <c r="D18" t="s">
+        <v>82</v>
+      </c>
+      <c r="E18" t="s">
         <v>172</v>
       </c>
-      <c r="D18" t="s">
-        <v>83</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>173</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>174</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>175</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
         <v>176</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" t="s">
         <v>177</v>
       </c>
-      <c r="J18" t="s">
-        <v>178</v>
-      </c>
       <c r="K18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L18">
         <v>23514</v>
@@ -1709,34 +1728,34 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C19" t="s">
+        <v>178</v>
+      </c>
+      <c r="D19" t="s">
         <v>179</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>180</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>181</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>182</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>183</v>
       </c>
-      <c r="H19" t="s">
+      <c r="I19" t="s">
         <v>184</v>
       </c>
-      <c r="I19" t="s">
+      <c r="J19" t="s">
         <v>185</v>
       </c>
-      <c r="J19" t="s">
-        <v>186</v>
-      </c>
       <c r="K19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L19">
         <v>94064</v>
@@ -1747,34 +1766,34 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C20" t="s">
+        <v>186</v>
+      </c>
+      <c r="D20" t="s">
         <v>187</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>188</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
+        <v>158</v>
+      </c>
+      <c r="G20" t="s">
         <v>189</v>
       </c>
-      <c r="F20" t="s">
-        <v>159</v>
-      </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>190</v>
       </c>
-      <c r="H20" t="s">
+      <c r="I20" t="s">
         <v>191</v>
       </c>
-      <c r="I20" t="s">
-        <v>192</v>
-      </c>
       <c r="J20" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L20">
         <v>92878</v>
@@ -1785,34 +1804,34 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C21" t="s">
+        <v>192</v>
+      </c>
+      <c r="D21" t="s">
         <v>193</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>194</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>195</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>196</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>197</v>
       </c>
-      <c r="H21" t="s">
+      <c r="I21" t="s">
         <v>198</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
         <v>199</v>
       </c>
-      <c r="J21" t="s">
-        <v>200</v>
-      </c>
       <c r="K21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L21">
         <v>50936</v>
@@ -1825,36 +1844,20 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1863,6 +1866,64 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="5.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
@@ -1889,38 +1950,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="7.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.7265625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1"/>
   <sheetViews>
@@ -1951,154 +1981,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="5.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.81640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="12.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.08984375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="8.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.81640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="5.54296875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="5.54296875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1"/>
   <sheetViews>
@@ -2129,7 +2012,38 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q1"/>
   <sheetViews>
@@ -2216,30 +2130,184 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="5.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C2" t="s">
+        <v>203</v>
+      </c>
+      <c r="D2" t="s">
+        <v>204</v>
+      </c>
+      <c r="E2" t="s">
+        <v>206</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D55" sqref="D55"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>250</v>
+      </c>
+      <c r="F2" s="1">
+        <v>42005</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
missing Shipment data, why? b/c wasn't 100% if it should be taken care of via sql referencing or manually inputed.
</commit_message>
<xml_diff>
--- a/src/data/seed.xlsx
+++ b/src/data/seed.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17088" windowHeight="5928" tabRatio="833" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17088" windowHeight="5928" tabRatio="833" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Account" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="274">
   <si>
     <t>customerId</t>
   </si>
@@ -857,6 +857,33 @@
   </si>
   <si>
     <t>public/images/parts/part6.jpg</t>
+  </si>
+  <si>
+    <t>USPS</t>
+  </si>
+  <si>
+    <t>FedEx</t>
+  </si>
+  <si>
+    <t>UPS</t>
+  </si>
+  <si>
+    <t>CanadaPost</t>
+  </si>
+  <si>
+    <t>Express</t>
+  </si>
+  <si>
+    <t>Overnight</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>Deliver between 08:00 and 20:00</t>
+  </si>
+  <si>
+    <t>If noone is home, leave out back</t>
   </si>
 </sst>
 </file>
@@ -5181,7 +5208,7 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5284,7 +5311,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5685,10 +5712,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q1"/>
+  <dimension ref="A1:Q18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5765,6 +5792,348 @@
         <v>27</v>
       </c>
     </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1000457</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>265</v>
+      </c>
+      <c r="D2" t="s">
+        <v>272</v>
+      </c>
+      <c r="E2">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="G2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <f>A2*2</f>
+        <v>2000914</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>268</v>
+      </c>
+      <c r="D3" t="s">
+        <v>273</v>
+      </c>
+      <c r="E3">
+        <v>123.45</v>
+      </c>
+      <c r="G3" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <f>A3*2</f>
+        <v>4001828</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>266</v>
+      </c>
+      <c r="D4" t="s">
+        <v>273</v>
+      </c>
+      <c r="E4">
+        <v>456.3</v>
+      </c>
+      <c r="G4" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>405002</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>265</v>
+      </c>
+      <c r="D5" t="s">
+        <v>272</v>
+      </c>
+      <c r="E5">
+        <v>32</v>
+      </c>
+      <c r="G5" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>253525</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>268</v>
+      </c>
+      <c r="D6" t="s">
+        <v>273</v>
+      </c>
+      <c r="E6">
+        <v>255.17500000000001</v>
+      </c>
+      <c r="G6" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>4653534</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>266</v>
+      </c>
+      <c r="D7" t="s">
+        <v>273</v>
+      </c>
+      <c r="E7">
+        <v>295.07499999999999</v>
+      </c>
+      <c r="G7" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>432442</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>265</v>
+      </c>
+      <c r="D8" t="s">
+        <v>273</v>
+      </c>
+      <c r="E8">
+        <v>334.97500000000002</v>
+      </c>
+      <c r="G8" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>432423</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>268</v>
+      </c>
+      <c r="D9" t="s">
+        <v>273</v>
+      </c>
+      <c r="E9">
+        <v>374.875</v>
+      </c>
+      <c r="G9" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>35435356</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>266</v>
+      </c>
+      <c r="D10" t="s">
+        <v>272</v>
+      </c>
+      <c r="E10">
+        <v>414.77499999999998</v>
+      </c>
+      <c r="G10" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>432465</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>265</v>
+      </c>
+      <c r="D11" t="s">
+        <v>272</v>
+      </c>
+      <c r="E11">
+        <v>454.67500000000001</v>
+      </c>
+      <c r="G11" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>353656</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>268</v>
+      </c>
+      <c r="D12" t="s">
+        <v>273</v>
+      </c>
+      <c r="E12">
+        <v>494.57499999999999</v>
+      </c>
+      <c r="G12" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>854</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>267</v>
+      </c>
+      <c r="D13" t="s">
+        <v>273</v>
+      </c>
+      <c r="E13">
+        <v>534.47500000000002</v>
+      </c>
+      <c r="G13" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>12325</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>265</v>
+      </c>
+      <c r="D14" t="s">
+        <v>272</v>
+      </c>
+      <c r="E14">
+        <v>574.375</v>
+      </c>
+      <c r="G14" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>533</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>268</v>
+      </c>
+      <c r="D15" t="s">
+        <v>273</v>
+      </c>
+      <c r="E15">
+        <v>614.27499999999998</v>
+      </c>
+      <c r="G15" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>53</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>267</v>
+      </c>
+      <c r="D16" t="s">
+        <v>272</v>
+      </c>
+      <c r="E16">
+        <v>654.17499999999995</v>
+      </c>
+      <c r="G16" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>525</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
+        <v>265</v>
+      </c>
+      <c r="D17" t="s">
+        <v>272</v>
+      </c>
+      <c r="E17">
+        <v>694.07500000000005</v>
+      </c>
+      <c r="G17" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>25252</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18" t="s">
+        <v>265</v>
+      </c>
+      <c r="D18" t="s">
+        <v>272</v>
+      </c>
+      <c r="E18">
+        <v>733.97500000000002</v>
+      </c>
+      <c r="G18" t="s">
+        <v>270</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5874,8 +6243,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6180,7 +6549,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6208,6 +6577,9 @@
       <c r="B2">
         <v>1</v>
       </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
@@ -6216,6 +6588,9 @@
       <c r="B3">
         <v>1</v>
       </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
@@ -6224,6 +6599,9 @@
       <c r="B4">
         <v>1</v>
       </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
@@ -6231,6 +6609,9 @@
       </c>
       <c r="B5">
         <v>2</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -6240,6 +6621,9 @@
       <c r="B6">
         <v>3</v>
       </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
@@ -6248,6 +6632,9 @@
       <c r="B7">
         <v>5</v>
       </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
@@ -6256,55 +6643,118 @@
       <c r="B8">
         <v>6</v>
       </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modify payment table and shipment table slightly
</commit_message>
<xml_diff>
--- a/src/data/seed.xlsx
+++ b/src/data/seed.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="327">
   <si>
     <t>accountId</t>
   </si>
@@ -61,6 +61,44 @@
     <t>postalCode</t>
   </si>
   <si>
+    <t>customer</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>test@test.com</t>
+    </r>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>1-(234)567-8900</t>
+  </si>
+  <si>
+    <t>1234 Fake St</t>
+  </si>
+  <si>
+    <t>Kelowna</t>
+  </si>
+  <si>
+    <t>British Columbia</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>A1A1A1</t>
+  </si>
+  <si>
     <t>admin</t>
   </si>
   <si>
@@ -136,9 +174,6 @@
     <t>5 Lerdahl Road</t>
   </si>
   <si>
-    <t>customer</t>
-  </si>
-  <si>
     <t>mhawkins3@shinystat.com</t>
   </si>
   <si>
@@ -568,21 +603,6 @@
     <t>toPostalCode</t>
   </si>
   <si>
-    <t>fromAddress</t>
-  </si>
-  <si>
-    <t>fromCity</t>
-  </si>
-  <si>
-    <t>fromProvinceState</t>
-  </si>
-  <si>
-    <t>fromCountry</t>
-  </si>
-  <si>
-    <t>fromPostalCode</t>
-  </si>
-  <si>
     <t>USPS</t>
   </si>
   <si>
@@ -601,15 +621,6 @@
     <t>Michigan</t>
   </si>
   <si>
-    <t>73331 Jana Way</t>
-  </si>
-  <si>
-    <t>Winston Salem</t>
-  </si>
-  <si>
-    <t>North Carolina</t>
-  </si>
-  <si>
     <t>CanadaPost</t>
   </si>
   <si>
@@ -628,69 +639,33 @@
     <t>Oklahoma</t>
   </si>
   <si>
-    <t>8888 Hoard Terrace</t>
-  </si>
-  <si>
-    <t>Dayton</t>
-  </si>
-  <si>
     <t>FedEx</t>
   </si>
   <si>
     <t>1 Shopko Court</t>
   </si>
   <si>
-    <t>51 Carioca Alley</t>
-  </si>
-  <si>
     <t>32 Autumn Leaf Court</t>
   </si>
   <si>
     <t>Rochester</t>
   </si>
   <si>
-    <t>00 1st Plaza</t>
-  </si>
-  <si>
-    <t>Dallas</t>
-  </si>
-  <si>
     <t>8343 Packers Hill</t>
   </si>
   <si>
-    <t>83 Browning Avenue</t>
-  </si>
-  <si>
-    <t>Lakewood</t>
-  </si>
-  <si>
     <t>85 Riverside Place</t>
   </si>
   <si>
     <t>Milwaukee</t>
   </si>
   <si>
-    <t>234 Hallows Alley</t>
-  </si>
-  <si>
-    <t>Sacramento</t>
-  </si>
-  <si>
     <t>92 Superior Avenue</t>
   </si>
   <si>
     <t>Johnson City</t>
   </si>
   <si>
-    <t>4 4th Plaza</t>
-  </si>
-  <si>
-    <t>Aurora</t>
-  </si>
-  <si>
-    <t>Colorado</t>
-  </si>
-  <si>
     <t>Overnight</t>
   </si>
   <si>
@@ -703,124 +678,61 @@
     <t>New Jersey</t>
   </si>
   <si>
-    <t>24168 Nelson Drive</t>
+    <t>10 Hagan Place</t>
   </si>
   <si>
     <t>Philadelphia</t>
   </si>
   <si>
-    <t>10 Hagan Place</t>
-  </si>
-  <si>
-    <t>29461 Logan Center</t>
-  </si>
-  <si>
-    <t>Atlanta</t>
+    <t>994 Fremont Road</t>
+  </si>
+  <si>
+    <t>Bradenton</t>
+  </si>
+  <si>
+    <t>33 Melody Center</t>
+  </si>
+  <si>
+    <t>El Paso</t>
+  </si>
+  <si>
+    <t>UPS</t>
+  </si>
+  <si>
+    <t>13133 Upham Way</t>
+  </si>
+  <si>
+    <t>Erie</t>
+  </si>
+  <si>
+    <t>194 Steensland Trail</t>
+  </si>
+  <si>
+    <t>Houston</t>
+  </si>
+  <si>
+    <t>26874 Bartelt Park</t>
+  </si>
+  <si>
+    <t>Roanoke</t>
+  </si>
+  <si>
+    <t>32 Buena Vista Park</t>
+  </si>
+  <si>
+    <t>Savannah</t>
   </si>
   <si>
     <t>Georgia</t>
   </si>
   <si>
-    <t>994 Fremont Road</t>
-  </si>
-  <si>
-    <t>Bradenton</t>
-  </si>
-  <si>
-    <t>90 Annamark Alley</t>
-  </si>
-  <si>
-    <t>Richmond</t>
-  </si>
-  <si>
-    <t>33 Melody Center</t>
-  </si>
-  <si>
-    <t>El Paso</t>
-  </si>
-  <si>
-    <t>74224 Jenna Trail</t>
-  </si>
-  <si>
-    <t>Arlington</t>
-  </si>
-  <si>
-    <t>UPS</t>
-  </si>
-  <si>
-    <t>13133 Upham Way</t>
-  </si>
-  <si>
-    <t>Erie</t>
-  </si>
-  <si>
-    <t>848 Lien Hill</t>
-  </si>
-  <si>
-    <t>Lake Charles</t>
-  </si>
-  <si>
-    <t>Louisiana</t>
-  </si>
-  <si>
-    <t>194 Steensland Trail</t>
-  </si>
-  <si>
-    <t>Houston</t>
-  </si>
-  <si>
-    <t>06327 Clyde Gallagher Center</t>
-  </si>
-  <si>
-    <t>Kansas City</t>
-  </si>
-  <si>
-    <t>Kansas</t>
-  </si>
-  <si>
-    <t>26874 Bartelt Park</t>
-  </si>
-  <si>
-    <t>Roanoke</t>
-  </si>
-  <si>
-    <t>49059 Dennis Terrace</t>
-  </si>
-  <si>
-    <t>32 Buena Vista Park</t>
-  </si>
-  <si>
-    <t>Savannah</t>
-  </si>
-  <si>
-    <t>0102 Hoepker Alley</t>
-  </si>
-  <si>
-    <t>Pueblo</t>
-  </si>
-  <si>
     <t>1 Debs Crossing</t>
   </si>
   <si>
-    <t>66075 Norway Maple Court</t>
-  </si>
-  <si>
-    <t>Waterbury</t>
-  </si>
-  <si>
-    <t>Connecticut</t>
-  </si>
-  <si>
     <t>9 Jackson Trail</t>
   </si>
   <si>
-    <t>3846 Westend Way</t>
-  </si>
-  <si>
-    <t>Albuquerque</t>
-  </si>
-  <si>
-    <t>New Mexico</t>
+    <t>paymentId</t>
   </si>
   <si>
     <t>accountNumber</t>
@@ -1109,7 +1021,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -1126,8 +1038,14 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <u val="single"/>
+      <sz val="11"/>
+      <color indexed="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <sz val="8"/>
-      <color indexed="11"/>
+      <color indexed="12"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -1145,7 +1063,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -1157,6 +1075,43 @@
       <left style="thin">
         <color indexed="10"/>
       </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="10"/>
       </right>
@@ -1211,7 +1166,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -1222,6 +1177,15 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -1245,25 +1209,25 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -1306,6 +1270,7 @@
       <rgbColor rgb="ff000000"/>
       <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ff0000ff"/>
       <rgbColor rgb="ff404040"/>
     </indexedColors>
   </colors>
@@ -2368,7 +2333,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -2431,38 +2396,38 @@
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="2">
+      <c r="B2" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="C2" t="s" s="2">
+      <c r="C2" t="s" s="5">
         <v>13</v>
       </c>
-      <c r="D2" t="s" s="2">
+      <c r="D2" t="s" s="5">
         <v>14</v>
       </c>
-      <c r="E2" t="s" s="2">
+      <c r="E2" t="s" s="5">
         <v>15</v>
       </c>
-      <c r="F2" t="s" s="2">
+      <c r="F2" t="s" s="5">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s" s="5">
         <v>16</v>
       </c>
-      <c r="G2" t="s" s="2">
+      <c r="H2" t="s" s="5">
         <v>17</v>
       </c>
-      <c r="H2" t="s" s="2">
+      <c r="I2" t="s" s="5">
         <v>18</v>
       </c>
-      <c r="I2" t="s" s="2">
+      <c r="J2" t="s" s="5">
         <v>19</v>
       </c>
-      <c r="J2" t="s" s="2">
+      <c r="K2" t="s" s="5">
         <v>20</v>
       </c>
-      <c r="K2" t="s" s="2">
+      <c r="L2" t="s" s="6">
         <v>21</v>
-      </c>
-      <c r="L2" s="3">
-        <v>20057</v>
       </c>
     </row>
     <row r="3" ht="15" customHeight="1">
@@ -2470,37 +2435,37 @@
         <v>2</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s" s="2">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E3" t="s" s="2">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F3" t="s" s="2">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G3" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H3" t="s" s="2">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I3" t="s" s="2">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J3" t="s" s="2">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K3" t="s" s="2">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="L3" s="3">
-        <v>12255</v>
+        <v>20057</v>
       </c>
     </row>
     <row r="4" ht="15" customHeight="1">
@@ -2508,37 +2473,37 @@
         <v>3</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="D4" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="E4" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="F4" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="G4" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="H4" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="I4" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="J4" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="K4" t="s" s="2">
         <v>31</v>
       </c>
-      <c r="D4" t="s" s="2">
-        <v>32</v>
-      </c>
-      <c r="E4" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="F4" t="s" s="2">
-        <v>34</v>
-      </c>
-      <c r="G4" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="H4" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="I4" t="s" s="2">
-        <v>28</v>
-      </c>
-      <c r="J4" t="s" s="2">
-        <v>29</v>
-      </c>
-      <c r="K4" t="s" s="2">
-        <v>21</v>
-      </c>
       <c r="L4" s="3">
-        <v>12237</v>
+        <v>12255</v>
       </c>
     </row>
     <row r="5" ht="15" customHeight="1">
@@ -2546,37 +2511,37 @@
         <v>4</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="D5" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="E5" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="F5" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="G5" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="H5" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="I5" t="s" s="2">
         <v>38</v>
       </c>
-      <c r="D5" t="s" s="2">
+      <c r="J5" t="s" s="2">
         <v>39</v>
       </c>
-      <c r="E5" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="F5" t="s" s="2">
-        <v>25</v>
-      </c>
-      <c r="G5" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="H5" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="I5" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="J5" t="s" s="2">
-        <v>44</v>
-      </c>
       <c r="K5" t="s" s="2">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="L5" s="3">
-        <v>33185</v>
+        <v>12237</v>
       </c>
     </row>
     <row r="6" ht="15" customHeight="1">
@@ -2584,37 +2549,37 @@
         <v>5</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s" s="2">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D6" t="s" s="2">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E6" t="s" s="2">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F6" t="s" s="2">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="G6" t="s" s="2">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H6" t="s" s="2">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I6" t="s" s="2">
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="J6" t="s" s="2">
-        <v>20</v>
+        <v>53</v>
       </c>
       <c r="K6" t="s" s="2">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="L6" s="3">
-        <v>20022</v>
+        <v>33185</v>
       </c>
     </row>
     <row r="7" ht="15" customHeight="1">
@@ -2622,37 +2587,37 @@
         <v>6</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s" s="2">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D7" t="s" s="2">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E7" t="s" s="2">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="F7" t="s" s="2">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="G7" t="s" s="2">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="H7" t="s" s="2">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="I7" t="s" s="2">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="J7" t="s" s="2">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="K7" t="s" s="2">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="L7" s="3">
-        <v>33467</v>
+        <v>20022</v>
       </c>
     </row>
     <row r="8" ht="15" customHeight="1">
@@ -2660,37 +2625,37 @@
         <v>7</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s" s="2">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D8" t="s" s="2">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E8" t="s" s="2">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="F8" t="s" s="2">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="G8" t="s" s="2">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H8" t="s" s="2">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I8" t="s" s="2">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="J8" t="s" s="2">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="K8" t="s" s="2">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="L8" s="3">
-        <v>75049</v>
+        <v>33467</v>
       </c>
     </row>
     <row r="9" ht="15" customHeight="1">
@@ -2698,37 +2663,37 @@
         <v>8</v>
       </c>
       <c r="B9" t="s" s="2">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s" s="2">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D9" t="s" s="2">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E9" t="s" s="2">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F9" t="s" s="2">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G9" t="s" s="2">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H9" t="s" s="2">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="I9" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J9" t="s" s="2">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="K9" t="s" s="2">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="L9" s="3">
-        <v>36622</v>
+        <v>75049</v>
       </c>
     </row>
     <row r="10" ht="15" customHeight="1">
@@ -2739,34 +2704,34 @@
         <v>12</v>
       </c>
       <c r="C10" t="s" s="2">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D10" t="s" s="2">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E10" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F10" t="s" s="2">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G10" t="s" s="2">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H10" t="s" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="I10" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J10" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="K10" t="s" s="2">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="L10" s="3">
-        <v>58122</v>
+        <v>36622</v>
       </c>
     </row>
     <row r="11" ht="15" customHeight="1">
@@ -2774,37 +2739,37 @@
         <v>10</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C11" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D11" t="s" s="2">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E11" t="s" s="2">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F11" t="s" s="2">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G11" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H11" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I11" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="J11" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="K11" t="s" s="2">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="L11" s="3">
-        <v>53779</v>
+        <v>58122</v>
       </c>
     </row>
     <row r="12" ht="15" customHeight="1">
@@ -2812,37 +2777,37 @@
         <v>11</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D12" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E12" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F12" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G12" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H12" t="s" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I12" t="s" s="2">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="J12" t="s" s="2">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="K12" t="s" s="2">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="L12" s="3">
-        <v>85715</v>
+        <v>53779</v>
       </c>
     </row>
     <row r="13" ht="15" customHeight="1">
@@ -2850,37 +2815,37 @@
         <v>12</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C13" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D13" t="s" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E13" t="s" s="2">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F13" t="s" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G13" t="s" s="2">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H13" t="s" s="2">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="I13" t="s" s="2">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="J13" t="s" s="2">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="K13" t="s" s="2">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="L13" s="3">
-        <v>38308</v>
+        <v>85715</v>
       </c>
     </row>
     <row r="14" ht="15" customHeight="1">
@@ -2888,37 +2853,37 @@
         <v>13</v>
       </c>
       <c r="B14" t="s" s="2">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="C14" t="s" s="2">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D14" t="s" s="2">
-        <v>52</v>
+        <v>108</v>
       </c>
       <c r="E14" t="s" s="2">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F14" t="s" s="2">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="G14" t="s" s="2">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="H14" t="s" s="2">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="I14" t="s" s="2">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="J14" t="s" s="2">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="K14" t="s" s="2">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="L14" s="3">
-        <v>45271</v>
+        <v>38308</v>
       </c>
     </row>
     <row r="15" ht="15" customHeight="1">
@@ -2926,37 +2891,37 @@
         <v>14</v>
       </c>
       <c r="B15" t="s" s="2">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="C15" t="s" s="2">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D15" t="s" s="2">
-        <v>114</v>
+        <v>61</v>
       </c>
       <c r="E15" t="s" s="2">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F15" t="s" s="2">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G15" t="s" s="2">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H15" t="s" s="2">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="I15" t="s" s="2">
-        <v>88</v>
+        <v>120</v>
       </c>
       <c r="J15" t="s" s="2">
-        <v>89</v>
+        <v>121</v>
       </c>
       <c r="K15" t="s" s="2">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="L15" s="3">
-        <v>53710</v>
+        <v>45271</v>
       </c>
     </row>
     <row r="16" ht="15" customHeight="1">
@@ -2964,37 +2929,37 @@
         <v>15</v>
       </c>
       <c r="B16" t="s" s="2">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="C16" t="s" s="2">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="D16" t="s" s="2">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="E16" t="s" s="2">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="F16" t="s" s="2">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="G16" t="s" s="2">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="H16" t="s" s="2">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="I16" t="s" s="2">
-        <v>125</v>
+        <v>97</v>
       </c>
       <c r="J16" t="s" s="2">
-        <v>126</v>
+        <v>98</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="L16" s="3">
-        <v>17622</v>
+        <v>53710</v>
       </c>
     </row>
     <row r="17" ht="15" customHeight="1">
@@ -3002,37 +2967,37 @@
         <v>16</v>
       </c>
       <c r="B17" t="s" s="2">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="C17" t="s" s="2">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D17" t="s" s="2">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E17" t="s" s="2">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F17" t="s" s="2">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="G17" t="s" s="2">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H17" t="s" s="2">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="I17" t="s" s="2">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="J17" t="s" s="2">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="L17" s="3">
-        <v>25775</v>
+        <v>17622</v>
       </c>
     </row>
     <row r="18" ht="15" customHeight="1">
@@ -3040,37 +3005,37 @@
         <v>17</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="C18" t="s" s="2">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D18" t="s" s="2">
-        <v>46</v>
+        <v>137</v>
       </c>
       <c r="E18" t="s" s="2">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F18" t="s" s="2">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="G18" t="s" s="2">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="H18" t="s" s="2">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="I18" t="s" s="2">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="J18" t="s" s="2">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="L18" s="3">
-        <v>23514</v>
+        <v>25775</v>
       </c>
     </row>
     <row r="19" ht="15" customHeight="1">
@@ -3078,37 +3043,37 @@
         <v>18</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="C19" t="s" s="2">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D19" t="s" s="2">
-        <v>143</v>
+        <v>55</v>
       </c>
       <c r="E19" t="s" s="2">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F19" t="s" s="2">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G19" t="s" s="2">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H19" t="s" s="2">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I19" t="s" s="2">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="J19" t="s" s="2">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="L19" s="3">
-        <v>94064</v>
+        <v>23514</v>
       </c>
     </row>
     <row r="20" ht="15" customHeight="1">
@@ -3116,37 +3081,37 @@
         <v>19</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="C20" t="s" s="2">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D20" t="s" s="2">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E20" t="s" s="2">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F20" t="s" s="2">
-        <v>122</v>
+        <v>154</v>
       </c>
       <c r="G20" t="s" s="2">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="H20" t="s" s="2">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="I20" t="s" s="2">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="J20" t="s" s="2">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="L20" s="3">
-        <v>92878</v>
+        <v>94064</v>
       </c>
     </row>
     <row r="21" ht="15" customHeight="1">
@@ -3154,40 +3119,81 @@
         <v>20</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="C21" t="s" s="2">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="D21" t="s" s="2">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="E21" t="s" s="2">
+        <v>161</v>
+      </c>
+      <c r="F21" t="s" s="2">
+        <v>131</v>
+      </c>
+      <c r="G21" t="s" s="2">
+        <v>162</v>
+      </c>
+      <c r="H21" t="s" s="2">
+        <v>163</v>
+      </c>
+      <c r="I21" t="s" s="2">
+        <v>164</v>
+      </c>
+      <c r="J21" t="s" s="2">
         <v>158</v>
       </c>
-      <c r="F21" t="s" s="2">
-        <v>159</v>
-      </c>
-      <c r="G21" t="s" s="2">
-        <v>160</v>
-      </c>
-      <c r="H21" t="s" s="2">
-        <v>161</v>
-      </c>
-      <c r="I21" t="s" s="2">
-        <v>162</v>
-      </c>
-      <c r="J21" t="s" s="2">
-        <v>163</v>
-      </c>
       <c r="K21" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="L21" s="3">
+        <v>92878</v>
+      </c>
+    </row>
+    <row r="22" ht="15" customHeight="1">
+      <c r="A22" s="3">
         <v>21</v>
       </c>
-      <c r="L21" s="3">
+      <c r="B22" t="s" s="2">
+        <v>22</v>
+      </c>
+      <c r="C22" t="s" s="2">
+        <v>165</v>
+      </c>
+      <c r="D22" t="s" s="2">
+        <v>166</v>
+      </c>
+      <c r="E22" t="s" s="2">
+        <v>167</v>
+      </c>
+      <c r="F22" t="s" s="2">
+        <v>168</v>
+      </c>
+      <c r="G22" t="s" s="2">
+        <v>169</v>
+      </c>
+      <c r="H22" t="s" s="2">
+        <v>170</v>
+      </c>
+      <c r="I22" t="s" s="2">
+        <v>171</v>
+      </c>
+      <c r="J22" t="s" s="2">
+        <v>172</v>
+      </c>
+      <c r="K22" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="L22" s="3">
         <v>50936</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" location="" tooltip="" display=""/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
@@ -3204,43 +3210,43 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="14.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="8.85156" style="21" customWidth="1"/>
-    <col min="2" max="256" width="8.85156" style="21" customWidth="1"/>
+    <col min="1" max="1" width="8.85156" style="24" customWidth="1"/>
+    <col min="2" max="256" width="8.85156" style="24" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>330</v>
+        <v>298</v>
       </c>
     </row>
     <row r="2" ht="15" customHeight="1">
       <c r="A2" t="s" s="2">
-        <v>331</v>
+        <v>299</v>
       </c>
     </row>
     <row r="3" ht="15" customHeight="1">
       <c r="A3" t="s" s="2">
-        <v>332</v>
+        <v>300</v>
       </c>
     </row>
     <row r="4" ht="15" customHeight="1">
       <c r="A4" t="s" s="2">
-        <v>333</v>
+        <v>301</v>
       </c>
     </row>
     <row r="5" ht="15" customHeight="1">
       <c r="A5" t="s" s="2">
-        <v>334</v>
+        <v>302</v>
       </c>
     </row>
     <row r="6" ht="15" customHeight="1">
       <c r="A6" t="s" s="2">
-        <v>335</v>
+        <v>303</v>
       </c>
     </row>
     <row r="7" ht="15" customHeight="1">
       <c r="A7" t="s" s="2">
-        <v>336</v>
+        <v>304</v>
       </c>
     </row>
   </sheetData>
@@ -3260,103 +3266,103 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="14.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="9.67188" style="22" customWidth="1"/>
-    <col min="2" max="256" width="8.85156" style="22" customWidth="1"/>
+    <col min="1" max="1" width="9.67188" style="25" customWidth="1"/>
+    <col min="2" max="256" width="8.85156" style="25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>330</v>
+        <v>298</v>
       </c>
     </row>
     <row r="2" ht="15" customHeight="1">
       <c r="A2" t="s" s="2">
-        <v>337</v>
+        <v>305</v>
       </c>
     </row>
     <row r="3" ht="15" customHeight="1">
       <c r="A3" t="s" s="2">
-        <v>338</v>
+        <v>306</v>
       </c>
     </row>
     <row r="4" ht="15" customHeight="1">
       <c r="A4" t="s" s="2">
-        <v>339</v>
+        <v>307</v>
       </c>
     </row>
     <row r="5" ht="15" customHeight="1">
       <c r="A5" t="s" s="2">
-        <v>340</v>
+        <v>308</v>
       </c>
     </row>
     <row r="6" ht="15" customHeight="1">
       <c r="A6" t="s" s="2">
-        <v>341</v>
+        <v>309</v>
       </c>
     </row>
     <row r="7" ht="15" customHeight="1">
       <c r="A7" t="s" s="2">
-        <v>342</v>
+        <v>310</v>
       </c>
     </row>
     <row r="8" ht="15" customHeight="1">
       <c r="A8" t="s" s="2">
-        <v>343</v>
+        <v>311</v>
       </c>
     </row>
     <row r="9" ht="15" customHeight="1">
       <c r="A9" t="s" s="2">
-        <v>344</v>
+        <v>312</v>
       </c>
     </row>
     <row r="10" ht="15" customHeight="1">
       <c r="A10" t="s" s="2">
-        <v>345</v>
+        <v>313</v>
       </c>
     </row>
     <row r="11" ht="15" customHeight="1">
       <c r="A11" t="s" s="2">
-        <v>346</v>
+        <v>314</v>
       </c>
     </row>
     <row r="12" ht="15" customHeight="1">
       <c r="A12" t="s" s="2">
-        <v>347</v>
+        <v>315</v>
       </c>
     </row>
     <row r="13" ht="15" customHeight="1">
       <c r="A13" t="s" s="2">
-        <v>348</v>
+        <v>316</v>
       </c>
     </row>
     <row r="14" ht="15" customHeight="1">
       <c r="A14" t="s" s="2">
-        <v>349</v>
+        <v>317</v>
       </c>
     </row>
     <row r="15" ht="15" customHeight="1">
       <c r="A15" t="s" s="2">
-        <v>350</v>
+        <v>318</v>
       </c>
     </row>
     <row r="16" ht="15" customHeight="1">
       <c r="A16" t="s" s="2">
-        <v>351</v>
+        <v>319</v>
       </c>
     </row>
     <row r="17" ht="15" customHeight="1">
       <c r="A17" t="s" s="2">
-        <v>352</v>
+        <v>320</v>
       </c>
     </row>
     <row r="18" ht="15" customHeight="1">
       <c r="A18" t="s" s="2">
-        <v>353</v>
+        <v>321</v>
       </c>
     </row>
     <row r="19" ht="15" customHeight="1">
       <c r="A19" t="s" s="2">
-        <v>354</v>
+        <v>322</v>
       </c>
     </row>
   </sheetData>
@@ -3376,25 +3382,25 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="14.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="8.17188" style="23" customWidth="1"/>
-    <col min="2" max="2" width="11.8516" style="23" customWidth="1"/>
-    <col min="3" max="3" width="12.5" style="23" customWidth="1"/>
-    <col min="4" max="4" width="5" style="23" customWidth="1"/>
-    <col min="5" max="256" width="8.85156" style="23" customWidth="1"/>
+    <col min="1" max="1" width="8.17188" style="26" customWidth="1"/>
+    <col min="2" max="2" width="11.8516" style="26" customWidth="1"/>
+    <col min="3" max="3" width="12.5" style="26" customWidth="1"/>
+    <col min="4" max="4" width="5" style="26" customWidth="1"/>
+    <col min="5" max="256" width="8.85156" style="26" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>355</v>
+        <v>323</v>
       </c>
       <c r="B1" t="s" s="2">
-        <v>356</v>
+        <v>324</v>
       </c>
       <c r="C1" t="s" s="2">
-        <v>357</v>
+        <v>325</v>
       </c>
       <c r="D1" t="s" s="2">
-        <v>358</v>
+        <v>326</v>
       </c>
     </row>
     <row r="2" ht="15" customHeight="1">
@@ -3402,10 +3408,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>331</v>
+        <v>299</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>337</v>
+        <v>305</v>
       </c>
       <c r="D2" s="3">
         <v>2008</v>
@@ -3416,10 +3422,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>331</v>
+        <v>299</v>
       </c>
       <c r="C3" t="s" s="2">
-        <v>337</v>
+        <v>305</v>
       </c>
       <c r="D3" s="3">
         <v>2009</v>
@@ -3430,10 +3436,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>331</v>
+        <v>299</v>
       </c>
       <c r="C4" t="s" s="2">
-        <v>337</v>
+        <v>305</v>
       </c>
       <c r="D4" s="3">
         <v>2010</v>
@@ -3444,10 +3450,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>331</v>
+        <v>299</v>
       </c>
       <c r="C5" t="s" s="2">
-        <v>338</v>
+        <v>306</v>
       </c>
       <c r="D5" s="3">
         <f>D2</f>
@@ -3459,10 +3465,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>331</v>
+        <v>299</v>
       </c>
       <c r="C6" t="s" s="2">
-        <v>338</v>
+        <v>306</v>
       </c>
       <c r="D6" s="3">
         <f>D3</f>
@@ -3474,10 +3480,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>331</v>
+        <v>299</v>
       </c>
       <c r="C7" t="s" s="2">
-        <v>338</v>
+        <v>306</v>
       </c>
       <c r="D7" s="3">
         <f>D4</f>
@@ -3489,10 +3495,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>333</v>
+        <v>301</v>
       </c>
       <c r="C8" t="s" s="2">
-        <v>339</v>
+        <v>307</v>
       </c>
       <c r="D8" s="3">
         <f>D5</f>
@@ -3504,10 +3510,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s" s="2">
-        <v>333</v>
+        <v>301</v>
       </c>
       <c r="C9" t="s" s="2">
-        <v>339</v>
+        <v>307</v>
       </c>
       <c r="D9" s="3">
         <f>D6</f>
@@ -3519,10 +3525,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>333</v>
+        <v>301</v>
       </c>
       <c r="C10" t="s" s="2">
-        <v>339</v>
+        <v>307</v>
       </c>
       <c r="D10" s="3">
         <f>D7</f>
@@ -3534,10 +3540,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>333</v>
+        <v>301</v>
       </c>
       <c r="C11" t="s" s="2">
-        <v>340</v>
+        <v>308</v>
       </c>
       <c r="D11" s="3">
         <f>D8</f>
@@ -3549,10 +3555,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>333</v>
+        <v>301</v>
       </c>
       <c r="C12" t="s" s="2">
-        <v>340</v>
+        <v>308</v>
       </c>
       <c r="D12" s="3">
         <f>D9</f>
@@ -3564,10 +3570,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>333</v>
+        <v>301</v>
       </c>
       <c r="C13" t="s" s="2">
-        <v>340</v>
+        <v>308</v>
       </c>
       <c r="D13" s="3">
         <f>D10</f>
@@ -3579,10 +3585,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s" s="2">
-        <v>332</v>
+        <v>300</v>
       </c>
       <c r="C14" t="s" s="2">
-        <v>342</v>
+        <v>310</v>
       </c>
       <c r="D14" s="3">
         <f>D11</f>
@@ -3594,10 +3600,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s" s="2">
-        <v>332</v>
+        <v>300</v>
       </c>
       <c r="C15" t="s" s="2">
-        <v>342</v>
+        <v>310</v>
       </c>
       <c r="D15" s="3">
         <f>D12</f>
@@ -3609,10 +3615,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s" s="2">
-        <v>332</v>
+        <v>300</v>
       </c>
       <c r="C16" t="s" s="2">
-        <v>342</v>
+        <v>310</v>
       </c>
       <c r="D16" s="3">
         <f>D13</f>
@@ -3624,10 +3630,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s" s="2">
-        <v>332</v>
+        <v>300</v>
       </c>
       <c r="C17" t="s" s="2">
-        <v>341</v>
+        <v>309</v>
       </c>
       <c r="D17" s="3">
         <f>D14</f>
@@ -3639,10 +3645,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>332</v>
+        <v>300</v>
       </c>
       <c r="C18" t="s" s="2">
-        <v>341</v>
+        <v>309</v>
       </c>
       <c r="D18" s="3">
         <f>D15</f>
@@ -3654,10 +3660,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>332</v>
+        <v>300</v>
       </c>
       <c r="C19" t="s" s="2">
-        <v>341</v>
+        <v>309</v>
       </c>
       <c r="D19" s="3">
         <f>D16</f>
@@ -3669,10 +3675,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>334</v>
+        <v>302</v>
       </c>
       <c r="C20" t="s" s="2">
-        <v>343</v>
+        <v>311</v>
       </c>
       <c r="D20" s="3">
         <f>D17</f>
@@ -3684,10 +3690,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>334</v>
+        <v>302</v>
       </c>
       <c r="C21" t="s" s="2">
-        <v>343</v>
+        <v>311</v>
       </c>
       <c r="D21" s="3">
         <f>D18</f>
@@ -3699,10 +3705,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>334</v>
+        <v>302</v>
       </c>
       <c r="C22" t="s" s="2">
-        <v>343</v>
+        <v>311</v>
       </c>
       <c r="D22" s="3">
         <f>D19</f>
@@ -3714,10 +3720,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>334</v>
+        <v>302</v>
       </c>
       <c r="C23" t="s" s="2">
-        <v>344</v>
+        <v>312</v>
       </c>
       <c r="D23" s="3">
         <f>D20</f>
@@ -3729,10 +3735,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>334</v>
+        <v>302</v>
       </c>
       <c r="C24" t="s" s="2">
-        <v>344</v>
+        <v>312</v>
       </c>
       <c r="D24" s="3">
         <f>D21</f>
@@ -3744,10 +3750,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>334</v>
+        <v>302</v>
       </c>
       <c r="C25" t="s" s="2">
-        <v>344</v>
+        <v>312</v>
       </c>
       <c r="D25" s="3">
         <f>D22</f>
@@ -3759,10 +3765,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>334</v>
+        <v>302</v>
       </c>
       <c r="C26" t="s" s="2">
-        <v>344</v>
+        <v>312</v>
       </c>
       <c r="D26" s="3">
         <v>2011</v>
@@ -3773,10 +3779,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>335</v>
+        <v>303</v>
       </c>
       <c r="C27" t="s" s="2">
-        <v>345</v>
+        <v>313</v>
       </c>
       <c r="D27" s="3">
         <f>D23</f>
@@ -3788,10 +3794,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>335</v>
+        <v>303</v>
       </c>
       <c r="C28" t="s" s="2">
-        <v>345</v>
+        <v>313</v>
       </c>
       <c r="D28" s="3">
         <f>D24</f>
@@ -3803,10 +3809,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>335</v>
+        <v>303</v>
       </c>
       <c r="C29" t="s" s="2">
-        <v>345</v>
+        <v>313</v>
       </c>
       <c r="D29" s="3">
         <f>D25</f>
@@ -3818,10 +3824,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>335</v>
+        <v>303</v>
       </c>
       <c r="C30" t="s" s="2">
-        <v>346</v>
+        <v>314</v>
       </c>
       <c r="D30" s="3">
         <f>D27</f>
@@ -3833,10 +3839,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>335</v>
+        <v>303</v>
       </c>
       <c r="C31" t="s" s="2">
-        <v>346</v>
+        <v>314</v>
       </c>
       <c r="D31" s="3">
         <f>D28</f>
@@ -3848,10 +3854,10 @@
         <v>31</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>335</v>
+        <v>303</v>
       </c>
       <c r="C32" t="s" s="2">
-        <v>346</v>
+        <v>314</v>
       </c>
       <c r="D32" s="3">
         <f>D29</f>
@@ -3863,10 +3869,10 @@
         <v>32</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>336</v>
+        <v>304</v>
       </c>
       <c r="C33" t="s" s="2">
-        <v>347</v>
+        <v>315</v>
       </c>
       <c r="D33" s="3">
         <f>D30</f>
@@ -3878,10 +3884,10 @@
         <v>33</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>336</v>
+        <v>304</v>
       </c>
       <c r="C34" t="s" s="2">
-        <v>347</v>
+        <v>315</v>
       </c>
       <c r="D34" s="3">
         <f>D31</f>
@@ -3893,10 +3899,10 @@
         <v>34</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>336</v>
+        <v>304</v>
       </c>
       <c r="C35" t="s" s="2">
-        <v>347</v>
+        <v>315</v>
       </c>
       <c r="D35" s="3">
         <f>D32</f>
@@ -3908,10 +3914,10 @@
         <v>35</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>336</v>
+        <v>304</v>
       </c>
       <c r="C36" t="s" s="2">
-        <v>348</v>
+        <v>316</v>
       </c>
       <c r="D36" s="3">
         <f>D33</f>
@@ -3923,10 +3929,10 @@
         <v>36</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>336</v>
+        <v>304</v>
       </c>
       <c r="C37" t="s" s="2">
-        <v>348</v>
+        <v>316</v>
       </c>
       <c r="D37" s="3">
         <f>D34</f>
@@ -3938,10 +3944,10 @@
         <v>37</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>336</v>
+        <v>304</v>
       </c>
       <c r="C38" t="s" s="2">
-        <v>348</v>
+        <v>316</v>
       </c>
       <c r="D38" s="3">
         <f>D35</f>
@@ -3953,10 +3959,10 @@
         <v>38</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>333</v>
+        <v>301</v>
       </c>
       <c r="C39" t="s" s="2">
-        <v>349</v>
+        <v>317</v>
       </c>
       <c r="D39" s="3">
         <v>2011</v>
@@ -3967,10 +3973,10 @@
         <v>39</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>333</v>
+        <v>301</v>
       </c>
       <c r="C40" t="s" s="2">
-        <v>349</v>
+        <v>317</v>
       </c>
       <c r="D40" s="3">
         <v>2012</v>
@@ -3981,10 +3987,10 @@
         <v>40</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>333</v>
+        <v>301</v>
       </c>
       <c r="C41" t="s" s="2">
-        <v>349</v>
+        <v>317</v>
       </c>
       <c r="D41" s="3">
         <v>2013</v>
@@ -3995,10 +4001,10 @@
         <v>41</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>333</v>
+        <v>301</v>
       </c>
       <c r="C42" t="s" s="2">
-        <v>350</v>
+        <v>318</v>
       </c>
       <c r="D42" s="3">
         <f>D39</f>
@@ -4010,10 +4016,10 @@
         <v>42</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>333</v>
+        <v>301</v>
       </c>
       <c r="C43" t="s" s="2">
-        <v>350</v>
+        <v>318</v>
       </c>
       <c r="D43" s="3">
         <f>D40</f>
@@ -4025,10 +4031,10 @@
         <v>43</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>333</v>
+        <v>301</v>
       </c>
       <c r="C44" t="s" s="2">
-        <v>350</v>
+        <v>318</v>
       </c>
       <c r="D44" s="3">
         <f>D41</f>
@@ -4040,10 +4046,10 @@
         <v>44</v>
       </c>
       <c r="B45" t="s" s="2">
-        <v>333</v>
+        <v>301</v>
       </c>
       <c r="C45" t="s" s="2">
-        <v>351</v>
+        <v>319</v>
       </c>
       <c r="D45" s="3">
         <f>D42</f>
@@ -4055,10 +4061,10 @@
         <v>45</v>
       </c>
       <c r="B46" t="s" s="2">
-        <v>333</v>
+        <v>301</v>
       </c>
       <c r="C46" t="s" s="2">
-        <v>351</v>
+        <v>319</v>
       </c>
       <c r="D46" s="3">
         <f>D43</f>
@@ -4070,10 +4076,10 @@
         <v>46</v>
       </c>
       <c r="B47" t="s" s="2">
-        <v>333</v>
+        <v>301</v>
       </c>
       <c r="C47" t="s" s="2">
-        <v>351</v>
+        <v>319</v>
       </c>
       <c r="D47" s="3">
         <f>D44</f>
@@ -4085,10 +4091,10 @@
         <v>47</v>
       </c>
       <c r="B48" t="s" s="2">
-        <v>333</v>
+        <v>301</v>
       </c>
       <c r="C48" t="s" s="2">
-        <v>352</v>
+        <v>320</v>
       </c>
       <c r="D48" s="3">
         <f>D45</f>
@@ -4100,10 +4106,10 @@
         <v>48</v>
       </c>
       <c r="B49" t="s" s="2">
-        <v>333</v>
+        <v>301</v>
       </c>
       <c r="C49" t="s" s="2">
-        <v>352</v>
+        <v>320</v>
       </c>
       <c r="D49" s="3">
         <f>D46</f>
@@ -4115,10 +4121,10 @@
         <v>49</v>
       </c>
       <c r="B50" t="s" s="2">
-        <v>333</v>
+        <v>301</v>
       </c>
       <c r="C50" t="s" s="2">
-        <v>352</v>
+        <v>320</v>
       </c>
       <c r="D50" s="3">
         <f>D47</f>
@@ -4130,10 +4136,10 @@
         <v>50</v>
       </c>
       <c r="B51" t="s" s="2">
-        <v>333</v>
+        <v>301</v>
       </c>
       <c r="C51" t="s" s="2">
-        <v>353</v>
+        <v>321</v>
       </c>
       <c r="D51" s="3">
         <f>D48</f>
@@ -4145,10 +4151,10 @@
         <v>51</v>
       </c>
       <c r="B52" t="s" s="2">
-        <v>333</v>
+        <v>301</v>
       </c>
       <c r="C52" t="s" s="2">
-        <v>353</v>
+        <v>321</v>
       </c>
       <c r="D52" s="3">
         <f>D49</f>
@@ -4160,10 +4166,10 @@
         <v>52</v>
       </c>
       <c r="B53" t="s" s="2">
-        <v>333</v>
+        <v>301</v>
       </c>
       <c r="C53" t="s" s="2">
-        <v>353</v>
+        <v>321</v>
       </c>
       <c r="D53" s="3">
         <f>D50</f>
@@ -4175,10 +4181,10 @@
         <v>53</v>
       </c>
       <c r="B54" t="s" s="2">
-        <v>333</v>
+        <v>301</v>
       </c>
       <c r="C54" t="s" s="2">
-        <v>354</v>
+        <v>322</v>
       </c>
       <c r="D54" s="3">
         <f>D51</f>
@@ -4190,10 +4196,10 @@
         <v>54</v>
       </c>
       <c r="B55" t="s" s="2">
-        <v>333</v>
+        <v>301</v>
       </c>
       <c r="C55" t="s" s="2">
-        <v>354</v>
+        <v>322</v>
       </c>
       <c r="D55" s="3">
         <f>D52</f>
@@ -4205,10 +4211,10 @@
         <v>55</v>
       </c>
       <c r="B56" t="s" s="2">
-        <v>333</v>
+        <v>301</v>
       </c>
       <c r="C56" t="s" s="2">
-        <v>354</v>
+        <v>322</v>
       </c>
       <c r="D56" s="3">
         <f>D53</f>
@@ -4232,17 +4238,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="14.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="5.85156" style="24" customWidth="1"/>
-    <col min="2" max="2" width="8.17188" style="24" customWidth="1"/>
-    <col min="3" max="256" width="8.85156" style="24" customWidth="1"/>
+    <col min="1" max="1" width="5.85156" style="27" customWidth="1"/>
+    <col min="2" max="2" width="8.17188" style="27" customWidth="1"/>
+    <col min="3" max="256" width="8.85156" style="27" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>291</v>
+        <v>259</v>
       </c>
       <c r="B1" t="s" s="2">
-        <v>355</v>
+        <v>323</v>
       </c>
     </row>
     <row r="2" ht="15" customHeight="1">
@@ -6382,21 +6388,21 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="14.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="10.1719" style="4" customWidth="1"/>
-    <col min="2" max="2" width="8.35156" style="4" customWidth="1"/>
-    <col min="3" max="3" width="9.67188" style="4" customWidth="1"/>
-    <col min="4" max="256" width="8.85156" style="4" customWidth="1"/>
+    <col min="1" max="1" width="10.1719" style="7" customWidth="1"/>
+    <col min="2" max="2" width="8.35156" style="7" customWidth="1"/>
+    <col min="3" max="3" width="9.67188" style="7" customWidth="1"/>
+    <col min="4" max="256" width="8.85156" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="B1" t="s" s="2">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="C1" t="s" s="2">
-        <v>166</v>
+        <v>175</v>
       </c>
     </row>
     <row r="2" ht="15" customHeight="1">
@@ -6482,21 +6488,21 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="14.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="7.17188" style="5" customWidth="1"/>
-    <col min="2" max="2" width="10.1719" style="5" customWidth="1"/>
-    <col min="3" max="3" width="9.35156" style="5" customWidth="1"/>
-    <col min="4" max="256" width="8.85156" style="5" customWidth="1"/>
+    <col min="1" max="1" width="7.17188" style="8" customWidth="1"/>
+    <col min="2" max="2" width="10.1719" style="8" customWidth="1"/>
+    <col min="3" max="3" width="9.35156" style="8" customWidth="1"/>
+    <col min="4" max="256" width="8.85156" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="B1" t="s" s="2">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="C1" t="s" s="2">
-        <v>168</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" ht="15" customHeight="1">
@@ -6506,7 +6512,7 @@
       <c r="B2" s="3">
         <v>1</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="9">
         <v>42005</v>
       </c>
     </row>
@@ -6517,7 +6523,7 @@
       <c r="B3" s="3">
         <v>2</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="9">
         <v>42006</v>
       </c>
     </row>
@@ -6528,7 +6534,7 @@
       <c r="B4" s="3">
         <v>2</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="9">
         <v>42007</v>
       </c>
     </row>
@@ -6539,7 +6545,7 @@
       <c r="B5" s="3">
         <v>2</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="9">
         <v>42008</v>
       </c>
     </row>
@@ -6550,7 +6556,7 @@
       <c r="B6" s="3">
         <v>1</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="9">
         <v>42009</v>
       </c>
     </row>
@@ -6561,7 +6567,7 @@
       <c r="B7" s="3">
         <v>4</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="9">
         <v>42010</v>
       </c>
     </row>
@@ -6572,7 +6578,7 @@
       <c r="B8" s="3">
         <v>5</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="9">
         <v>42011</v>
       </c>
     </row>
@@ -6583,7 +6589,7 @@
       <c r="B9" s="3">
         <v>1</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="9">
         <v>42012</v>
       </c>
     </row>
@@ -6594,7 +6600,7 @@
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="9">
         <v>42013</v>
       </c>
     </row>
@@ -6605,7 +6611,7 @@
       <c r="B11" s="3">
         <v>2</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="9">
         <v>42014</v>
       </c>
     </row>
@@ -6616,7 +6622,7 @@
       <c r="B12" s="3">
         <v>4</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="9">
         <v>42015</v>
       </c>
     </row>
@@ -6627,7 +6633,7 @@
       <c r="B13" s="3">
         <v>5</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="9">
         <v>42016</v>
       </c>
     </row>
@@ -6638,7 +6644,7 @@
       <c r="B14" s="3">
         <v>5</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="9">
         <v>42017</v>
       </c>
     </row>
@@ -6649,7 +6655,7 @@
       <c r="B15" s="3">
         <v>5</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="9">
         <v>42018</v>
       </c>
     </row>
@@ -6660,7 +6666,7 @@
       <c r="B16" s="3">
         <v>5</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="9">
         <v>42019</v>
       </c>
     </row>
@@ -6671,7 +6677,7 @@
       <c r="B17" s="3">
         <v>5</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="9">
         <v>42020</v>
       </c>
     </row>
@@ -6682,7 +6688,7 @@
       <c r="B18" s="3">
         <v>1</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="9">
         <v>42021</v>
       </c>
     </row>
@@ -6697,87 +6703,67 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:R18"/>
+  <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="14.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="14.1719" style="7" customWidth="1"/>
-    <col min="2" max="2" width="14.1719" style="7" customWidth="1"/>
-    <col min="3" max="3" width="7.17188" style="7" customWidth="1"/>
-    <col min="4" max="4" width="6.17188" style="7" customWidth="1"/>
-    <col min="5" max="5" width="9.85156" style="7" customWidth="1"/>
-    <col min="6" max="6" width="7.85156" style="7" customWidth="1"/>
-    <col min="7" max="7" width="13.5" style="7" customWidth="1"/>
-    <col min="8" max="8" width="10" style="7" customWidth="1"/>
-    <col min="9" max="9" width="9.17188" style="7" customWidth="1"/>
-    <col min="10" max="10" width="5.67188" style="7" customWidth="1"/>
-    <col min="11" max="11" width="13.8516" style="7" customWidth="1"/>
-    <col min="12" max="12" width="9.17188" style="7" customWidth="1"/>
-    <col min="13" max="13" width="11.8516" style="7" customWidth="1"/>
-    <col min="14" max="14" width="11.6719" style="7" customWidth="1"/>
-    <col min="15" max="15" width="8" style="7" customWidth="1"/>
-    <col min="16" max="16" width="16.1719" style="7" customWidth="1"/>
-    <col min="17" max="17" width="11.5" style="7" customWidth="1"/>
-    <col min="18" max="18" width="14.1719" style="7" customWidth="1"/>
-    <col min="19" max="256" width="8.85156" style="7" customWidth="1"/>
+    <col min="1" max="1" width="14.1719" style="10" customWidth="1"/>
+    <col min="2" max="2" width="14.1719" style="10" customWidth="1"/>
+    <col min="3" max="3" width="7.17188" style="10" customWidth="1"/>
+    <col min="4" max="4" width="6.17188" style="10" customWidth="1"/>
+    <col min="5" max="5" width="9.85156" style="10" customWidth="1"/>
+    <col min="6" max="6" width="7.85156" style="10" customWidth="1"/>
+    <col min="7" max="7" width="13.5" style="10" customWidth="1"/>
+    <col min="8" max="8" width="10" style="10" customWidth="1"/>
+    <col min="9" max="9" width="9.17188" style="10" customWidth="1"/>
+    <col min="10" max="10" width="5.67188" style="10" customWidth="1"/>
+    <col min="11" max="11" width="13.8516" style="10" customWidth="1"/>
+    <col min="12" max="12" width="9.17188" style="10" customWidth="1"/>
+    <col min="13" max="13" width="11.8516" style="10" customWidth="1"/>
+    <col min="14" max="256" width="8.85156" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>169</v>
+        <v>178</v>
       </c>
       <c r="B1" t="s" s="2">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="C1" t="s" s="2">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="D1" t="s" s="2">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="E1" t="s" s="2">
-        <v>172</v>
+        <v>181</v>
       </c>
       <c r="F1" t="s" s="2">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="G1" t="s" s="2">
-        <v>174</v>
+        <v>183</v>
       </c>
       <c r="H1" t="s" s="2">
-        <v>175</v>
+        <v>184</v>
       </c>
       <c r="I1" t="s" s="2">
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="J1" t="s" s="2">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="K1" t="s" s="2">
-        <v>178</v>
+        <v>187</v>
       </c>
       <c r="L1" t="s" s="2">
-        <v>179</v>
+        <v>188</v>
       </c>
       <c r="M1" t="s" s="2">
-        <v>180</v>
-      </c>
-      <c r="N1" t="s" s="2">
-        <v>181</v>
-      </c>
-      <c r="O1" t="s" s="2">
-        <v>182</v>
-      </c>
-      <c r="P1" t="s" s="2">
-        <v>183</v>
-      </c>
-      <c r="Q1" t="s" s="2">
-        <v>184</v>
-      </c>
-      <c r="R1" t="s" s="2">
-        <v>185</v>
+        <v>189</v>
       </c>
     </row>
     <row r="2" ht="15" customHeight="1">
@@ -6791,49 +6777,34 @@
         <v>1</v>
       </c>
       <c r="D2" t="s" s="2">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="E2" t="s" s="2">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="F2" s="3">
         <v>9.949999999999999</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="9">
         <v>42005</v>
       </c>
       <c r="H2" t="s" s="2">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="I2" t="s" s="2">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="J2" t="s" s="2">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="K2" t="s" s="2">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="L2" t="s" s="2">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="M2" s="3">
         <v>48335</v>
-      </c>
-      <c r="N2" t="s" s="2">
-        <v>192</v>
-      </c>
-      <c r="O2" t="s" s="2">
-        <v>193</v>
-      </c>
-      <c r="P2" t="s" s="2">
-        <v>194</v>
-      </c>
-      <c r="Q2" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="R2" s="3">
-        <v>27116</v>
       </c>
     </row>
     <row r="3" ht="15" customHeight="1">
@@ -6848,49 +6819,34 @@
         <v>2</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E3" t="s" s="2">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F3" s="3">
         <v>123.45</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="9">
         <v>42006</v>
       </c>
       <c r="H3" t="s" s="2">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="I3" t="s" s="2">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="J3" t="s" s="2">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="K3" t="s" s="2">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="L3" t="s" s="2">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="M3" s="3">
         <v>74133</v>
-      </c>
-      <c r="N3" t="s" s="2">
-        <v>201</v>
-      </c>
-      <c r="O3" t="s" s="2">
-        <v>202</v>
-      </c>
-      <c r="P3" t="s" s="2">
-        <v>112</v>
-      </c>
-      <c r="Q3" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="R3" s="3">
-        <v>45440</v>
       </c>
     </row>
     <row r="4" ht="15" customHeight="1">
@@ -6905,49 +6861,34 @@
         <v>3</v>
       </c>
       <c r="D4" t="s" s="2">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E4" t="s" s="2">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F4" s="3">
         <v>456.3</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="9">
         <v>42007</v>
       </c>
       <c r="H4" t="s" s="2">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="I4" t="s" s="2">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J4" t="s" s="2">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="K4" t="s" s="2">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="L4" t="s" s="2">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="M4" s="3">
         <v>85754</v>
-      </c>
-      <c r="N4" t="s" s="2">
-        <v>205</v>
-      </c>
-      <c r="O4" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="P4" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Q4" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="R4" s="3">
-        <v>20337</v>
       </c>
     </row>
     <row r="5" ht="15" customHeight="1">
@@ -6961,49 +6902,34 @@
         <v>4</v>
       </c>
       <c r="D5" t="s" s="2">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="E5" t="s" s="2">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="F5" s="3">
         <v>32</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="9">
         <v>42008</v>
       </c>
       <c r="H5" t="s" s="2">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="I5" t="s" s="2">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="J5" t="s" s="2">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="K5" t="s" s="2">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="L5" t="s" s="2">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="M5" s="3">
         <v>14652</v>
-      </c>
-      <c r="N5" t="s" s="2">
-        <v>208</v>
-      </c>
-      <c r="O5" t="s" s="2">
-        <v>209</v>
-      </c>
-      <c r="P5" t="s" s="2">
-        <v>65</v>
-      </c>
-      <c r="Q5" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="R5" s="3">
-        <v>75236</v>
       </c>
     </row>
     <row r="6" ht="15" customHeight="1">
@@ -7017,49 +6943,34 @@
         <v>5</v>
       </c>
       <c r="D6" t="s" s="2">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E6" t="s" s="2">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F6" s="3">
         <v>255.175</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="9">
         <v>42009</v>
       </c>
       <c r="H6" t="s" s="2">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="I6" t="s" s="2">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="J6" t="s" s="2">
-        <v>162</v>
+        <v>171</v>
       </c>
       <c r="K6" t="s" s="2">
-        <v>163</v>
+        <v>172</v>
       </c>
       <c r="L6" t="s" s="2">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="M6" s="3">
         <v>50320</v>
-      </c>
-      <c r="N6" t="s" s="2">
-        <v>211</v>
-      </c>
-      <c r="O6" t="s" s="2">
-        <v>212</v>
-      </c>
-      <c r="P6" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="Q6" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="R6" s="3">
-        <v>98498</v>
       </c>
     </row>
     <row r="7" ht="15" customHeight="1">
@@ -7073,49 +6984,34 @@
         <v>6</v>
       </c>
       <c r="D7" t="s" s="2">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E7" t="s" s="2">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F7" s="3">
         <v>295.075</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="9">
         <v>42010</v>
       </c>
       <c r="H7" t="s" s="2">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="I7" t="s" s="2">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="J7" t="s" s="2">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="K7" t="s" s="2">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="L7" t="s" s="2">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="M7" s="3">
         <v>53215</v>
-      </c>
-      <c r="N7" t="s" s="2">
-        <v>215</v>
-      </c>
-      <c r="O7" t="s" s="2">
-        <v>216</v>
-      </c>
-      <c r="P7" t="s" s="2">
-        <v>149</v>
-      </c>
-      <c r="Q7" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="R7" s="3">
-        <v>95852</v>
       </c>
     </row>
     <row r="8" ht="15" customHeight="1">
@@ -7129,49 +7025,34 @@
         <v>7</v>
       </c>
       <c r="D8" t="s" s="2">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="E8" t="s" s="2">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F8" s="3">
         <v>334.975</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="9">
         <v>42011</v>
       </c>
       <c r="H8" t="s" s="2">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="I8" t="s" s="2">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="J8" t="s" s="2">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="K8" t="s" s="2">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="L8" t="s" s="2">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="M8" s="3">
         <v>37605</v>
-      </c>
-      <c r="N8" t="s" s="2">
-        <v>219</v>
-      </c>
-      <c r="O8" t="s" s="2">
-        <v>220</v>
-      </c>
-      <c r="P8" t="s" s="2">
-        <v>221</v>
-      </c>
-      <c r="Q8" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="R8" s="3">
-        <v>80045</v>
       </c>
     </row>
     <row r="9" ht="15" customHeight="1">
@@ -7185,49 +7066,34 @@
         <v>8</v>
       </c>
       <c r="D9" t="s" s="2">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E9" t="s" s="2">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F9" s="3">
         <v>374.875</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="9">
         <v>42012</v>
       </c>
       <c r="H9" t="s" s="2">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="I9" t="s" s="2">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="J9" t="s" s="2">
-        <v>224</v>
+        <v>213</v>
       </c>
       <c r="K9" t="s" s="2">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="L9" t="s" s="2">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="M9" s="3">
         <v>8104</v>
-      </c>
-      <c r="N9" t="s" s="2">
-        <v>226</v>
-      </c>
-      <c r="O9" t="s" s="2">
-        <v>227</v>
-      </c>
-      <c r="P9" t="s" s="2">
-        <v>126</v>
-      </c>
-      <c r="Q9" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="R9" s="3">
-        <v>19093</v>
       </c>
     </row>
     <row r="10" ht="15" customHeight="1">
@@ -7241,49 +7107,34 @@
         <v>9</v>
       </c>
       <c r="D10" t="s" s="2">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E10" t="s" s="2">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="F10" s="3">
         <v>414.775</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="9">
         <v>42013</v>
       </c>
       <c r="H10" t="s" s="2">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="I10" t="s" s="2">
-        <v>228</v>
+        <v>215</v>
       </c>
       <c r="J10" t="s" s="2">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="K10" t="s" s="2">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="L10" t="s" s="2">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="M10" s="3">
         <v>19172</v>
-      </c>
-      <c r="N10" t="s" s="2">
-        <v>229</v>
-      </c>
-      <c r="O10" t="s" s="2">
-        <v>230</v>
-      </c>
-      <c r="P10" t="s" s="2">
-        <v>231</v>
-      </c>
-      <c r="Q10" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="R10" s="3">
-        <v>30311</v>
       </c>
     </row>
     <row r="11" ht="15" customHeight="1">
@@ -7297,49 +7148,34 @@
         <v>10</v>
       </c>
       <c r="D11" t="s" s="2">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="E11" t="s" s="2">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="F11" s="3">
         <v>454.675</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G11" s="9">
         <v>42014</v>
       </c>
       <c r="H11" t="s" s="2">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="I11" t="s" s="2">
-        <v>232</v>
+        <v>217</v>
       </c>
       <c r="J11" t="s" s="2">
-        <v>233</v>
+        <v>218</v>
       </c>
       <c r="K11" t="s" s="2">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="L11" t="s" s="2">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="M11" s="3">
         <v>34282</v>
-      </c>
-      <c r="N11" t="s" s="2">
-        <v>234</v>
-      </c>
-      <c r="O11" t="s" s="2">
-        <v>235</v>
-      </c>
-      <c r="P11" t="s" s="2">
-        <v>141</v>
-      </c>
-      <c r="Q11" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="R11" s="3">
-        <v>23213</v>
       </c>
     </row>
     <row r="12" ht="15" customHeight="1">
@@ -7353,49 +7189,34 @@
         <v>11</v>
       </c>
       <c r="D12" t="s" s="2">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E12" t="s" s="2">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F12" s="3">
         <v>494.575</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="9">
         <v>42015</v>
       </c>
       <c r="H12" t="s" s="2">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="I12" t="s" s="2">
-        <v>236</v>
+        <v>219</v>
       </c>
       <c r="J12" t="s" s="2">
-        <v>237</v>
+        <v>220</v>
       </c>
       <c r="K12" t="s" s="2">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="L12" t="s" s="2">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="M12" s="3">
         <v>88563</v>
-      </c>
-      <c r="N12" t="s" s="2">
-        <v>238</v>
-      </c>
-      <c r="O12" t="s" s="2">
-        <v>239</v>
-      </c>
-      <c r="P12" t="s" s="2">
-        <v>141</v>
-      </c>
-      <c r="Q12" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="R12" s="3">
-        <v>22244</v>
       </c>
     </row>
     <row r="13" ht="15" customHeight="1">
@@ -7409,49 +7230,34 @@
         <v>12</v>
       </c>
       <c r="D13" t="s" s="2">
-        <v>240</v>
+        <v>221</v>
       </c>
       <c r="E13" t="s" s="2">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F13" s="3">
         <v>534.475</v>
       </c>
-      <c r="G13" s="6">
+      <c r="G13" s="9">
         <v>42016</v>
       </c>
       <c r="H13" t="s" s="2">
+        <v>211</v>
+      </c>
+      <c r="I13" t="s" s="2">
         <v>222</v>
       </c>
-      <c r="I13" t="s" s="2">
-        <v>241</v>
-      </c>
       <c r="J13" t="s" s="2">
-        <v>242</v>
+        <v>223</v>
       </c>
       <c r="K13" t="s" s="2">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="L13" t="s" s="2">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="M13" s="3">
         <v>16565</v>
-      </c>
-      <c r="N13" t="s" s="2">
-        <v>243</v>
-      </c>
-      <c r="O13" t="s" s="2">
-        <v>244</v>
-      </c>
-      <c r="P13" t="s" s="2">
-        <v>245</v>
-      </c>
-      <c r="Q13" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="R13" s="3">
-        <v>70616</v>
       </c>
     </row>
     <row r="14" ht="15" customHeight="1">
@@ -7465,49 +7271,34 @@
         <v>13</v>
       </c>
       <c r="D14" t="s" s="2">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="E14" t="s" s="2">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="F14" s="3">
         <v>574.375</v>
       </c>
-      <c r="G14" s="6">
+      <c r="G14" s="9">
         <v>42017</v>
       </c>
       <c r="H14" t="s" s="2">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="I14" t="s" s="2">
-        <v>246</v>
+        <v>224</v>
       </c>
       <c r="J14" t="s" s="2">
-        <v>247</v>
+        <v>225</v>
       </c>
       <c r="K14" t="s" s="2">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="M14" s="3">
         <v>77010</v>
-      </c>
-      <c r="N14" t="s" s="2">
-        <v>248</v>
-      </c>
-      <c r="O14" t="s" s="2">
-        <v>249</v>
-      </c>
-      <c r="P14" t="s" s="2">
-        <v>250</v>
-      </c>
-      <c r="Q14" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="R14" s="3">
-        <v>66112</v>
       </c>
     </row>
     <row r="15" ht="15" customHeight="1">
@@ -7521,49 +7312,34 @@
         <v>14</v>
       </c>
       <c r="D15" t="s" s="2">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E15" t="s" s="2">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F15" s="3">
         <v>614.275</v>
       </c>
-      <c r="G15" s="6">
+      <c r="G15" s="9">
         <v>42018</v>
       </c>
       <c r="H15" t="s" s="2">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="I15" t="s" s="2">
-        <v>251</v>
+        <v>226</v>
       </c>
       <c r="J15" t="s" s="2">
-        <v>252</v>
+        <v>227</v>
       </c>
       <c r="K15" t="s" s="2">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="M15" s="3">
         <v>24040</v>
-      </c>
-      <c r="N15" t="s" s="2">
-        <v>253</v>
-      </c>
-      <c r="O15" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="P15" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Q15" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="R15" s="3">
-        <v>56944</v>
       </c>
     </row>
     <row r="16" ht="15" customHeight="1">
@@ -7577,49 +7353,34 @@
         <v>15</v>
       </c>
       <c r="D16" t="s" s="2">
-        <v>240</v>
+        <v>221</v>
       </c>
       <c r="E16" t="s" s="2">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="F16" s="3">
         <v>654.175</v>
       </c>
-      <c r="G16" s="6">
+      <c r="G16" s="9">
         <v>42019</v>
       </c>
       <c r="H16" t="s" s="2">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="I16" t="s" s="2">
-        <v>254</v>
+        <v>228</v>
       </c>
       <c r="J16" t="s" s="2">
-        <v>255</v>
+        <v>229</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="M16" s="3">
         <v>31416</v>
-      </c>
-      <c r="N16" t="s" s="2">
-        <v>256</v>
-      </c>
-      <c r="O16" t="s" s="2">
-        <v>257</v>
-      </c>
-      <c r="P16" t="s" s="2">
-        <v>221</v>
-      </c>
-      <c r="Q16" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="R16" s="3">
-        <v>81005</v>
       </c>
     </row>
     <row r="17" ht="15" customHeight="1">
@@ -7633,49 +7394,34 @@
         <v>16</v>
       </c>
       <c r="D17" t="s" s="2">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="E17" t="s" s="2">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="F17" s="3">
         <v>694.075</v>
       </c>
-      <c r="G17" s="6">
+      <c r="G17" s="9">
         <v>42020</v>
       </c>
       <c r="H17" t="s" s="2">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="I17" t="s" s="2">
-        <v>258</v>
+        <v>231</v>
       </c>
       <c r="J17" t="s" s="2">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="M17" s="3">
         <v>20520</v>
-      </c>
-      <c r="N17" t="s" s="2">
-        <v>259</v>
-      </c>
-      <c r="O17" t="s" s="2">
-        <v>260</v>
-      </c>
-      <c r="P17" t="s" s="2">
-        <v>261</v>
-      </c>
-      <c r="Q17" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="R17" s="3">
-        <v>6726</v>
       </c>
     </row>
     <row r="18" ht="15" customHeight="1">
@@ -7689,49 +7435,34 @@
         <v>17</v>
       </c>
       <c r="D18" t="s" s="2">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="E18" t="s" s="2">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="F18" s="3">
         <v>733.975</v>
       </c>
-      <c r="G18" s="6">
+      <c r="G18" s="9">
         <v>42021</v>
       </c>
       <c r="H18" t="s" s="2">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="I18" t="s" s="2">
-        <v>262</v>
+        <v>232</v>
       </c>
       <c r="J18" t="s" s="2">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="M18" s="3">
         <v>20540</v>
-      </c>
-      <c r="N18" t="s" s="2">
-        <v>263</v>
-      </c>
-      <c r="O18" t="s" s="2">
-        <v>264</v>
-      </c>
-      <c r="P18" t="s" s="2">
-        <v>265</v>
-      </c>
-      <c r="Q18" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="R18" s="3">
-        <v>87115</v>
       </c>
     </row>
   </sheetData>
@@ -7745,27 +7476,31 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="14.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="14.1719" style="8" customWidth="1"/>
-    <col min="2" max="2" width="10.1719" style="8" customWidth="1"/>
-    <col min="3" max="3" width="12.1719" style="8" customWidth="1"/>
-    <col min="4" max="256" width="8.85156" style="8" customWidth="1"/>
+    <col min="1" max="1" width="14.1719" style="11" customWidth="1"/>
+    <col min="2" max="2" width="10.1719" style="11" customWidth="1"/>
+    <col min="3" max="3" width="14.1719" style="11" customWidth="1"/>
+    <col min="4" max="4" width="12.1719" style="11" customWidth="1"/>
+    <col min="5" max="256" width="8.85156" style="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>266</v>
+        <v>233</v>
       </c>
       <c r="B1" t="s" s="2">
-        <v>169</v>
+        <v>178</v>
       </c>
       <c r="C1" t="s" s="2">
-        <v>267</v>
+        <v>234</v>
+      </c>
+      <c r="D1" t="s" s="2">
+        <v>235</v>
       </c>
     </row>
     <row r="2" ht="15" customHeight="1">
@@ -7775,8 +7510,11 @@
       <c r="B2" s="3">
         <v>1</v>
       </c>
-      <c r="C2" t="s" s="2">
-        <v>268</v>
+      <c r="C2" s="3">
+        <v>847182374</v>
+      </c>
+      <c r="D2" t="s" s="2">
+        <v>236</v>
       </c>
     </row>
     <row r="3" ht="15" customHeight="1">
@@ -7786,140 +7524,179 @@
       <c r="B3" s="3">
         <v>2</v>
       </c>
-      <c r="C3" t="s" s="2">
-        <v>268</v>
+      <c r="C3" s="3">
+        <v>192347918</v>
+      </c>
+      <c r="D3" t="s" s="2">
+        <v>236</v>
       </c>
     </row>
     <row r="4" ht="15" customHeight="1">
       <c r="A4" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="3">
         <v>3</v>
       </c>
-      <c r="C4" t="s" s="2">
-        <v>269</v>
+      <c r="C4" s="3">
+        <v>754823793</v>
+      </c>
+      <c r="D4" t="s" s="2">
+        <v>237</v>
       </c>
     </row>
     <row r="5" ht="15" customHeight="1">
       <c r="A5" s="3">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B5" s="3">
         <v>4</v>
       </c>
-      <c r="C5" t="s" s="2">
-        <v>269</v>
+      <c r="C5" s="3">
+        <v>234524352</v>
+      </c>
+      <c r="D5" t="s" s="2">
+        <v>237</v>
       </c>
     </row>
     <row r="6" ht="15" customHeight="1">
       <c r="A6" s="3">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B6" s="3">
         <v>5</v>
       </c>
-      <c r="C6" t="s" s="2">
-        <v>268</v>
+      <c r="C6" s="3">
+        <v>764324547</v>
+      </c>
+      <c r="D6" t="s" s="2">
+        <v>236</v>
       </c>
     </row>
     <row r="7" ht="15" customHeight="1">
       <c r="A7" s="3">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B7" s="3">
         <v>6</v>
       </c>
-      <c r="C7" t="s" s="2">
-        <v>269</v>
+      <c r="C7" s="3">
+        <v>424527744</v>
+      </c>
+      <c r="D7" t="s" s="2">
+        <v>237</v>
       </c>
     </row>
     <row r="8" ht="15" customHeight="1">
       <c r="A8" s="3">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B8" s="3">
         <v>7</v>
       </c>
-      <c r="C8" t="s" s="2">
-        <v>270</v>
+      <c r="C8" s="3">
+        <v>134468533</v>
+      </c>
+      <c r="D8" t="s" s="2">
+        <v>238</v>
       </c>
     </row>
     <row r="9" ht="15" customHeight="1">
       <c r="A9" s="3">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B9" s="3">
         <v>8</v>
       </c>
-      <c r="C9" t="s" s="2">
-        <v>268</v>
+      <c r="C9" s="3">
+        <v>354678578</v>
+      </c>
+      <c r="D9" t="s" s="2">
+        <v>236</v>
       </c>
     </row>
     <row r="10" ht="15" customHeight="1">
       <c r="A10" s="3">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B10" s="3">
         <v>9</v>
       </c>
-      <c r="C10" t="s" s="2">
-        <v>270</v>
+      <c r="C10" s="3">
+        <v>135426547</v>
+      </c>
+      <c r="D10" t="s" s="2">
+        <v>238</v>
       </c>
     </row>
     <row r="11" ht="15" customHeight="1">
       <c r="A11" s="3">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B11" s="3">
         <v>10</v>
       </c>
-      <c r="C11" t="s" s="2">
-        <v>269</v>
+      <c r="C11" s="3">
+        <v>345667687</v>
+      </c>
+      <c r="D11" t="s" s="2">
+        <v>237</v>
       </c>
     </row>
     <row r="12" ht="15" customHeight="1">
       <c r="A12" s="3">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B12" s="3">
         <v>11</v>
       </c>
-      <c r="C12" t="s" s="2">
-        <v>268</v>
+      <c r="C12" s="3">
+        <v>234524677</v>
+      </c>
+      <c r="D12" t="s" s="2">
+        <v>236</v>
       </c>
     </row>
     <row r="13" ht="15" customHeight="1">
       <c r="A13" s="3">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B13" s="3">
         <v>12</v>
       </c>
-      <c r="C13" t="s" s="2">
-        <v>270</v>
+      <c r="C13" s="3">
+        <v>444563788</v>
+      </c>
+      <c r="D13" t="s" s="2">
+        <v>238</v>
       </c>
     </row>
     <row r="14" ht="15" customHeight="1">
       <c r="A14" s="3">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B14" s="3">
         <v>13</v>
       </c>
-      <c r="C14" t="s" s="2">
-        <v>268</v>
+      <c r="C14" s="3">
+        <v>536875654</v>
+      </c>
+      <c r="D14" t="s" s="2">
+        <v>236</v>
       </c>
     </row>
     <row r="15" ht="15" customHeight="1">
       <c r="A15" s="3">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B15" s="3">
         <v>14</v>
       </c>
-      <c r="C15" t="s" s="2">
-        <v>270</v>
+      <c r="C15" s="3">
+        <v>456745689</v>
+      </c>
+      <c r="D15" t="s" s="2">
+        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -7939,89 +7716,89 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="14.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="12.8516" style="9" customWidth="1"/>
-    <col min="2" max="2" width="105.172" style="9" customWidth="1"/>
-    <col min="3" max="256" width="8.85156" style="9" customWidth="1"/>
+    <col min="1" max="1" width="12.8516" style="12" customWidth="1"/>
+    <col min="2" max="2" width="105.172" style="12" customWidth="1"/>
+    <col min="3" max="256" width="8.85156" style="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>271</v>
+        <v>239</v>
       </c>
       <c r="B1" t="s" s="2">
-        <v>272</v>
+        <v>240</v>
       </c>
     </row>
     <row r="2" ht="15" customHeight="1">
       <c r="A2" t="s" s="2">
-        <v>273</v>
+        <v>241</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>274</v>
+        <v>242</v>
       </c>
     </row>
     <row r="3" ht="15" customHeight="1">
       <c r="A3" t="s" s="2">
-        <v>275</v>
+        <v>243</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>276</v>
+        <v>244</v>
       </c>
     </row>
     <row r="4" ht="15" customHeight="1">
       <c r="A4" t="s" s="2">
-        <v>277</v>
+        <v>245</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>278</v>
+        <v>246</v>
       </c>
     </row>
     <row r="5" ht="15" customHeight="1">
       <c r="A5" t="s" s="2">
-        <v>279</v>
+        <v>247</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>280</v>
+        <v>248</v>
       </c>
     </row>
     <row r="6" ht="15" customHeight="1">
       <c r="A6" t="s" s="2">
-        <v>281</v>
+        <v>249</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>282</v>
+        <v>250</v>
       </c>
     </row>
     <row r="7" ht="15" customHeight="1">
       <c r="A7" t="s" s="2">
-        <v>283</v>
+        <v>251</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>284</v>
+        <v>252</v>
       </c>
     </row>
     <row r="8" ht="15" customHeight="1">
       <c r="A8" t="s" s="2">
-        <v>285</v>
+        <v>253</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>286</v>
+        <v>254</v>
       </c>
     </row>
     <row r="9" ht="15" customHeight="1">
       <c r="A9" t="s" s="2">
-        <v>287</v>
+        <v>255</v>
       </c>
       <c r="B9" t="s" s="2">
-        <v>288</v>
+        <v>256</v>
       </c>
     </row>
     <row r="10" ht="15" customHeight="1">
       <c r="A10" t="s" s="2">
-        <v>289</v>
+        <v>257</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>290</v>
+        <v>258</v>
       </c>
     </row>
   </sheetData>
@@ -8041,29 +7818,29 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="14.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="5.85156" style="10" customWidth="1"/>
-    <col min="2" max="2" width="12.8516" style="10" customWidth="1"/>
-    <col min="3" max="3" width="21.5" style="10" customWidth="1"/>
-    <col min="4" max="4" width="93.3516" style="10" customWidth="1"/>
-    <col min="5" max="5" width="26.3516" style="10" customWidth="1"/>
-    <col min="6" max="256" width="8.85156" style="10" customWidth="1"/>
+    <col min="1" max="1" width="5.85156" style="13" customWidth="1"/>
+    <col min="2" max="2" width="12.8516" style="13" customWidth="1"/>
+    <col min="3" max="3" width="21.5" style="13" customWidth="1"/>
+    <col min="4" max="4" width="93.3516" style="13" customWidth="1"/>
+    <col min="5" max="5" width="26.3516" style="13" customWidth="1"/>
+    <col min="6" max="256" width="8.85156" style="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>291</v>
+        <v>259</v>
       </c>
       <c r="B1" t="s" s="2">
-        <v>271</v>
+        <v>239</v>
       </c>
       <c r="C1" t="s" s="2">
-        <v>292</v>
+        <v>260</v>
       </c>
       <c r="D1" t="s" s="2">
-        <v>272</v>
+        <v>240</v>
       </c>
       <c r="E1" t="s" s="2">
-        <v>293</v>
+        <v>261</v>
       </c>
     </row>
     <row r="2" ht="15" customHeight="1">
@@ -8071,16 +7848,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>273</v>
+        <v>241</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>294</v>
+        <v>262</v>
       </c>
       <c r="D2" t="s" s="2">
-        <v>295</v>
+        <v>263</v>
       </c>
       <c r="E2" t="s" s="2">
-        <v>296</v>
+        <v>264</v>
       </c>
     </row>
     <row r="3" ht="15" customHeight="1">
@@ -8088,16 +7865,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>275</v>
+        <v>243</v>
       </c>
       <c r="C3" t="s" s="2">
-        <v>297</v>
+        <v>265</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>298</v>
+        <v>266</v>
       </c>
       <c r="E3" t="s" s="2">
-        <v>299</v>
+        <v>267</v>
       </c>
     </row>
     <row r="4" ht="15" customHeight="1">
@@ -8105,16 +7882,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>300</v>
+        <v>268</v>
       </c>
       <c r="C4" t="s" s="2">
-        <v>301</v>
+        <v>269</v>
       </c>
       <c r="D4" t="s" s="2">
-        <v>298</v>
+        <v>266</v>
       </c>
       <c r="E4" t="s" s="2">
-        <v>302</v>
+        <v>270</v>
       </c>
     </row>
     <row r="5" ht="15" customHeight="1">
@@ -8122,16 +7899,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>275</v>
+        <v>243</v>
       </c>
       <c r="C5" t="s" s="2">
-        <v>303</v>
+        <v>271</v>
       </c>
       <c r="D5" t="s" s="2">
-        <v>304</v>
+        <v>272</v>
       </c>
       <c r="E5" t="s" s="2">
-        <v>305</v>
+        <v>273</v>
       </c>
     </row>
     <row r="6" ht="15" customHeight="1">
@@ -8139,16 +7916,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>289</v>
+        <v>257</v>
       </c>
       <c r="C6" t="s" s="2">
-        <v>306</v>
+        <v>274</v>
       </c>
       <c r="D6" t="s" s="2">
-        <v>307</v>
+        <v>275</v>
       </c>
       <c r="E6" t="s" s="2">
-        <v>308</v>
+        <v>276</v>
       </c>
     </row>
     <row r="7" ht="15" customHeight="1">
@@ -8156,67 +7933,67 @@
         <v>6</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>289</v>
+        <v>257</v>
       </c>
       <c r="C7" t="s" s="2">
-        <v>309</v>
+        <v>277</v>
       </c>
       <c r="D7" t="s" s="2">
-        <v>310</v>
+        <v>278</v>
       </c>
       <c r="E7" t="s" s="2">
-        <v>311</v>
+        <v>279</v>
       </c>
     </row>
     <row r="8" ht="14.4" customHeight="1">
-      <c r="A8" s="11">
+      <c r="A8" s="14">
         <v>7</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>277</v>
-      </c>
-      <c r="C8" t="s" s="12">
-        <v>312</v>
-      </c>
-      <c r="D8" t="s" s="13">
-        <v>313</v>
+        <v>245</v>
+      </c>
+      <c r="C8" t="s" s="15">
+        <v>280</v>
+      </c>
+      <c r="D8" t="s" s="16">
+        <v>281</v>
       </c>
       <c r="E8" t="s" s="2">
-        <v>314</v>
+        <v>282</v>
       </c>
     </row>
     <row r="9" ht="14.4" customHeight="1">
-      <c r="A9" s="14">
+      <c r="A9" s="17">
         <v>8</v>
       </c>
       <c r="B9" t="s" s="2">
-        <v>279</v>
-      </c>
-      <c r="C9" t="s" s="15">
-        <v>315</v>
-      </c>
-      <c r="D9" t="s" s="15">
-        <v>280</v>
+        <v>247</v>
+      </c>
+      <c r="C9" t="s" s="18">
+        <v>283</v>
+      </c>
+      <c r="D9" t="s" s="18">
+        <v>248</v>
       </c>
       <c r="E9" t="s" s="2">
-        <v>316</v>
+        <v>284</v>
       </c>
     </row>
     <row r="10" ht="14.4" customHeight="1">
-      <c r="A10" s="16">
+      <c r="A10" s="19">
         <v>9</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>281</v>
-      </c>
-      <c r="C10" t="s" s="15">
-        <v>317</v>
-      </c>
-      <c r="D10" t="s" s="15">
-        <v>282</v>
+        <v>249</v>
+      </c>
+      <c r="C10" t="s" s="18">
+        <v>285</v>
+      </c>
+      <c r="D10" t="s" s="18">
+        <v>250</v>
       </c>
       <c r="E10" t="s" s="2">
-        <v>318</v>
+        <v>286</v>
       </c>
     </row>
     <row r="11" ht="14.4" customHeight="1">
@@ -8224,16 +8001,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>283</v>
-      </c>
-      <c r="C11" t="s" s="15">
-        <v>319</v>
-      </c>
-      <c r="D11" t="s" s="15">
-        <v>284</v>
+        <v>251</v>
+      </c>
+      <c r="C11" t="s" s="18">
+        <v>287</v>
+      </c>
+      <c r="D11" t="s" s="18">
+        <v>252</v>
       </c>
       <c r="E11" t="s" s="2">
-        <v>320</v>
+        <v>288</v>
       </c>
     </row>
     <row r="12" ht="14.4" customHeight="1">
@@ -8241,16 +8018,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>285</v>
-      </c>
-      <c r="C12" t="s" s="15">
-        <v>321</v>
-      </c>
-      <c r="D12" t="s" s="15">
-        <v>322</v>
+        <v>253</v>
+      </c>
+      <c r="C12" t="s" s="18">
+        <v>289</v>
+      </c>
+      <c r="D12" t="s" s="18">
+        <v>290</v>
       </c>
       <c r="E12" t="s" s="2">
-        <v>323</v>
+        <v>291</v>
       </c>
     </row>
     <row r="13" ht="14.4" customHeight="1">
@@ -8258,16 +8035,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>287</v>
-      </c>
-      <c r="C13" t="s" s="17">
-        <v>324</v>
-      </c>
-      <c r="D13" t="s" s="17">
-        <v>288</v>
+        <v>255</v>
+      </c>
+      <c r="C13" t="s" s="20">
+        <v>292</v>
+      </c>
+      <c r="D13" t="s" s="20">
+        <v>256</v>
       </c>
       <c r="E13" t="s" s="2">
-        <v>325</v>
+        <v>293</v>
       </c>
     </row>
   </sheetData>
@@ -8287,33 +8064,33 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="14.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="4.85156" style="18" customWidth="1"/>
-    <col min="2" max="2" width="8.35156" style="18" customWidth="1"/>
-    <col min="3" max="3" width="5.85156" style="18" customWidth="1"/>
-    <col min="4" max="4" width="7.85156" style="18" customWidth="1"/>
-    <col min="5" max="5" width="4.85156" style="18" customWidth="1"/>
-    <col min="6" max="6" width="9.35156" style="18" customWidth="1"/>
-    <col min="7" max="256" width="8.85156" style="18" customWidth="1"/>
+    <col min="1" max="1" width="4.85156" style="21" customWidth="1"/>
+    <col min="2" max="2" width="8.35156" style="21" customWidth="1"/>
+    <col min="3" max="3" width="5.85156" style="21" customWidth="1"/>
+    <col min="4" max="4" width="7.85156" style="21" customWidth="1"/>
+    <col min="5" max="5" width="4.85156" style="21" customWidth="1"/>
+    <col min="6" max="6" width="9.35156" style="21" customWidth="1"/>
+    <col min="7" max="256" width="8.85156" style="21" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>326</v>
+        <v>294</v>
       </c>
       <c r="B1" t="s" s="2">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="C1" t="s" s="2">
-        <v>291</v>
+        <v>259</v>
       </c>
       <c r="D1" t="s" s="2">
-        <v>327</v>
+        <v>295</v>
       </c>
       <c r="E1" t="s" s="2">
-        <v>328</v>
+        <v>296</v>
       </c>
       <c r="F1" t="s" s="2">
-        <v>329</v>
+        <v>297</v>
       </c>
     </row>
     <row r="2" ht="15" customHeight="1">
@@ -8332,7 +8109,7 @@
       <c r="E2" s="3">
         <v>250</v>
       </c>
-      <c r="F2" s="19">
+      <c r="F2" s="22">
         <v>42005</v>
       </c>
     </row>
@@ -8352,7 +8129,7 @@
       <c r="E3" s="3">
         <v>100</v>
       </c>
-      <c r="F3" s="19">
+      <c r="F3" s="22">
         <v>42006</v>
       </c>
     </row>
@@ -8372,7 +8149,7 @@
       <c r="E4" s="3">
         <v>100</v>
       </c>
-      <c r="F4" s="19">
+      <c r="F4" s="22">
         <v>42007</v>
       </c>
     </row>
@@ -8392,7 +8169,7 @@
       <c r="E5" s="3">
         <v>120</v>
       </c>
-      <c r="F5" s="19">
+      <c r="F5" s="22">
         <v>42008</v>
       </c>
     </row>
@@ -8412,7 +8189,7 @@
       <c r="E6" s="3">
         <v>600</v>
       </c>
-      <c r="F6" s="19">
+      <c r="F6" s="22">
         <v>42009</v>
       </c>
     </row>
@@ -8432,7 +8209,7 @@
       <c r="E7" s="3">
         <v>500</v>
       </c>
-      <c r="F7" s="19">
+      <c r="F7" s="22">
         <v>42010</v>
       </c>
     </row>
@@ -8453,21 +8230,21 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="14.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="7.17188" style="20" customWidth="1"/>
-    <col min="2" max="2" width="4.85156" style="20" customWidth="1"/>
-    <col min="3" max="3" width="7.85156" style="20" customWidth="1"/>
-    <col min="4" max="256" width="8.85156" style="20" customWidth="1"/>
+    <col min="1" max="1" width="7.17188" style="23" customWidth="1"/>
+    <col min="2" max="2" width="4.85156" style="23" customWidth="1"/>
+    <col min="3" max="3" width="7.85156" style="23" customWidth="1"/>
+    <col min="4" max="256" width="8.85156" style="23" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="B1" t="s" s="2">
-        <v>326</v>
+        <v>294</v>
       </c>
       <c r="C1" t="s" s="2">
-        <v>327</v>
+        <v>295</v>
       </c>
     </row>
     <row r="2" ht="15" customHeight="1">

</xml_diff>

<commit_message>
Change seed listed part quantities
</commit_message>
<xml_diff>
--- a/src/data/seed.xlsx
+++ b/src/data/seed.xlsx
@@ -8104,7 +8104,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="3">
-        <v>1</v>
+        <v>500</v>
       </c>
       <c r="E2" s="3">
         <v>250</v>
@@ -8124,7 +8124,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="3">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E3" s="3">
         <v>100</v>
@@ -8144,7 +8144,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="3">
-        <v>1</v>
+        <v>500</v>
       </c>
       <c r="E4" s="3">
         <v>100</v>
@@ -8164,7 +8164,7 @@
         <v>4</v>
       </c>
       <c r="D5" s="3">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="E5" s="3">
         <v>120</v>
@@ -8184,7 +8184,7 @@
         <v>6</v>
       </c>
       <c r="D6" s="3">
-        <v>1</v>
+        <v>900</v>
       </c>
       <c r="E6" s="3">
         <v>600</v>
@@ -8204,7 +8204,7 @@
         <v>5</v>
       </c>
       <c r="D7" s="3">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="E7" s="3">
         <v>500</v>

</xml_diff>